<commit_message>
Break out old week 2.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27040" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curriculum" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="158">
   <si>
     <t>Wk#</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Th</t>
   </si>
   <si>
-    <t>In-class ME</t>
-  </si>
-  <si>
     <t>Assignment</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>Agile, Testing, Debugging</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Know Thy Error Message, know the class of things stored in your variables</t>
   </si>
   <si>
@@ -106,39 +100,21 @@
     <t>Battleship</t>
   </si>
   <si>
-    <t>How to Google, read documentation</t>
-  </si>
-  <si>
-    <t>Agile, Draw more.</t>
-  </si>
-  <si>
     <t>Methods</t>
   </si>
   <si>
     <t>Database</t>
   </si>
   <si>
-    <t>Control Flow (next, break, etc)</t>
-  </si>
-  <si>
     <t>Databases</t>
   </si>
   <si>
     <t>Skinny Models</t>
   </si>
   <si>
-    <t>Reading</t>
-  </si>
-  <si>
-    <t>Assignment begs the question of</t>
-  </si>
-  <si>
     <t>http://blog.codeclimate.com/blog/2012/10/17/7-ways-to-decompose-fat-activerecord-models/</t>
   </si>
   <si>
-    <t>Debugging, Estimating</t>
-  </si>
-  <si>
     <t>Estimating Games PDF</t>
   </si>
   <si>
@@ -424,29 +400,107 @@
     <t>Nested Joins</t>
   </si>
   <si>
-    <t>Git Topics</t>
-  </si>
-  <si>
     <t>init, clone, add, commit, push</t>
   </si>
   <si>
-    <t>Control Flow and Variables</t>
-  </si>
-  <si>
-    <t>Methods and Arrays</t>
-  </si>
-  <si>
-    <t>Hashes and Nested Data Structures</t>
-  </si>
-  <si>
     <t>Classes</t>
+  </si>
+  <si>
+    <t>Git</t>
+  </si>
+  <si>
+    <t>Human Learning</t>
+  </si>
+  <si>
+    <t>Estimating</t>
+  </si>
+  <si>
+    <t>Googling</t>
+  </si>
+  <si>
+    <t>Enumerables</t>
+  </si>
+  <si>
+    <t>Enumerables, Inheritance</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Reading Docs</t>
+  </si>
+  <si>
+    <t>3 ZONES</t>
+  </si>
+  <si>
+    <t>AGILE</t>
+  </si>
+  <si>
+    <t>Testing, Exceptions</t>
+  </si>
+  <si>
+    <t>Composition, Modules</t>
+  </si>
+  <si>
+    <t>branch, pull</t>
+  </si>
+  <si>
+    <t>Pair Programming</t>
+  </si>
+  <si>
+    <t>HTML, CSS</t>
+  </si>
+  <si>
+    <t>Rails, MVC</t>
+  </si>
+  <si>
+    <t>Control Flow, Variables</t>
+  </si>
+  <si>
+    <t>Methods, Arrays</t>
+  </si>
+  <si>
+    <t>Hashes, Nested Data Structures</t>
+  </si>
+  <si>
+    <t>Assignment leads to</t>
+  </si>
+  <si>
+    <t>next, break, return, exit</t>
+  </si>
+  <si>
+    <t>Currency Converter</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Gemfile, Git</t>
+  </si>
+  <si>
+    <t>NILM</t>
+  </si>
+  <si>
+    <t>Ping-pong Pairing</t>
+  </si>
+  <si>
+    <t>CSS Reverse Engineer</t>
+  </si>
+  <si>
+    <t>Personal Site</t>
+  </si>
+  <si>
+    <t>Motivating Ex.</t>
+  </si>
+  <si>
+    <t>Reading/Listening</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -485,6 +539,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFA6A6A6"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -503,7 +569,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -541,13 +607,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -566,6 +648,13 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -584,6 +673,13 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -913,25 +1009,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="5.1640625" customWidth="1"/>
     <col min="3" max="3" width="4.5" customWidth="1"/>
-    <col min="4" max="5" width="31.83203125" customWidth="1"/>
-    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -945,220 +1046,301 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
       <c r="I1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>147</v>
+      </c>
+      <c r="J1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
         <v>136</v>
       </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="G4" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E5" t="s">
-        <v>135</v>
+        <v>145</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>146</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>127</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>138</v>
+      </c>
+      <c r="F10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>133</v>
+      </c>
+      <c r="F11" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>139</v>
+      </c>
+      <c r="F12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>151</v>
+      </c>
+      <c r="E13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="C17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="F17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="C18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="F18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="C19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="F19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="C22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="C24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:8">
       <c r="C25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="C28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="C29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:8">
       <c r="C30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:8">
       <c r="C31" t="s">
         <v>7</v>
       </c>
@@ -1168,7 +1350,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1196,7 +1378,7 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1209,7 +1391,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1227,7 +1409,7 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1245,55 +1427,55 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:10">
       <c r="C49" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:10">
       <c r="C52" t="s">
         <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>34</v>
-      </c>
-      <c r="I52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>29</v>
+      </c>
+      <c r="J52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="C53" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:10">
       <c r="C54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:10">
       <c r="C55" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:10">
       <c r="B57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="B59" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="B58" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="B59" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1324,433 +1506,433 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
         <v>71</v>
-      </c>
-      <c r="B17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B32" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C41" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Break out old week 3.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="172">
   <si>
     <t>Wk#</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Models &amp; DB</t>
   </si>
   <si>
-    <t>Agile, Testing, Debugging</t>
-  </si>
-  <si>
     <t>Know Thy Error Message, know the class of things stored in your variables</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Controllers &amp; APIs</t>
   </si>
   <si>
-    <t>ActiveModel Serializers</t>
-  </si>
-  <si>
     <t>PB&amp;J</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>Databases</t>
-  </si>
-  <si>
     <t>Skinny Models</t>
   </si>
   <si>
@@ -451,9 +442,6 @@
     <t>HTML, CSS</t>
   </si>
   <si>
-    <t>Rails, MVC</t>
-  </si>
-  <si>
     <t>Control Flow, Variables</t>
   </si>
   <si>
@@ -475,9 +463,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Gemfile, Git</t>
-  </si>
-  <si>
     <t>NILM</t>
   </si>
   <si>
@@ -494,6 +479,63 @@
   </si>
   <si>
     <t>Reading/Listening</t>
+  </si>
+  <si>
+    <t>Agile, Testing</t>
+  </si>
+  <si>
+    <t>Gemfile, TDD</t>
+  </si>
+  <si>
+    <t>Employees and Depts?</t>
+  </si>
+  <si>
+    <t>Motivational Quotations</t>
+  </si>
+  <si>
+    <t>Regex, ActiveModel Serializers</t>
+  </si>
+  <si>
+    <t>Rails, Web, HTML Verbs</t>
+  </si>
+  <si>
+    <t>Router, Controllers</t>
+  </si>
+  <si>
+    <t>HTML Forms, ERB</t>
+  </si>
+  <si>
+    <t>Emp &amp; Dept in Database</t>
+  </si>
+  <si>
+    <t>Data Diagrams (many)</t>
+  </si>
+  <si>
+    <t>Wallet</t>
+  </si>
+  <si>
+    <t>Databases, Migrations</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>Make-your-own API</t>
+  </si>
+  <si>
+    <t>Dev vs. Prod, Heroku</t>
+  </si>
+  <si>
+    <t>ActiveRecord, Dev vs. Test</t>
+  </si>
+  <si>
+    <t>Associations, Validations</t>
+  </si>
+  <si>
+    <t>Health Tracker</t>
+  </si>
+  <si>
+    <t>Scaffold, Helpers/Partials</t>
   </si>
 </sst>
 </file>
@@ -569,8 +611,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -629,7 +677,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -655,6 +703,9 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -680,6 +731,9 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1015,7 +1069,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1046,25 +1100,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1080,19 +1134,19 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1100,19 +1154,19 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1120,13 +1174,13 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1134,16 +1188,16 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1151,7 +1205,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1159,19 +1213,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -1179,19 +1233,19 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -1199,19 +1253,19 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1219,19 +1273,22 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G13" t="s">
-        <v>140</v>
+        <v>137</v>
+      </c>
+      <c r="H13" t="s">
+        <v>155</v>
       </c>
       <c r="I13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1247,23 +1304,38 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>164</v>
+      </c>
+      <c r="F16" t="s">
+        <v>165</v>
+      </c>
+      <c r="H16" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="C17" t="s">
         <v>5</v>
       </c>
+      <c r="D17" t="s">
+        <v>168</v>
+      </c>
       <c r="F17" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="H17" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="C18" t="s">
         <v>6</v>
       </c>
+      <c r="D18" t="s">
+        <v>169</v>
+      </c>
       <c r="F18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1271,7 +1343,7 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1279,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1287,7 +1359,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1295,18 +1367,27 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="C24" t="s">
         <v>6</v>
       </c>
+      <c r="D24" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="C25" t="s">
         <v>7</v>
       </c>
+      <c r="D25" t="s">
+        <v>167</v>
+      </c>
+      <c r="H25" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
@@ -1321,29 +1402,44 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E28" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H28" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="C29" t="s">
         <v>5</v>
       </c>
+      <c r="D29" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="C30" t="s">
         <v>6</v>
       </c>
+      <c r="D30" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="C31" t="s">
         <v>7</v>
       </c>
+      <c r="H31" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
@@ -1378,7 +1474,7 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1391,7 +1487,7 @@
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1409,7 +1505,7 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1442,10 +1538,10 @@
         <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J52" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -1465,17 +1561,17 @@
     </row>
     <row r="57" spans="1:10">
       <c r="B57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="B58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="B59" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1506,433 +1602,433 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
         <v>61</v>
       </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
         <v>59</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B55" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Break out old week 4.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -19,8 +19,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Mason</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mason:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Deploy to Heroku</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mason:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Existing Codebase</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="186">
   <si>
     <t>Wk#</t>
   </si>
@@ -64,24 +122,12 @@
     <t>Know Thy Error Message, know the class of things stored in your variables</t>
   </si>
   <si>
-    <t>APIs</t>
-  </si>
-  <si>
     <t>Legacy Code</t>
   </si>
   <si>
-    <t>Exceptions</t>
-  </si>
-  <si>
-    <t>Estimates</t>
-  </si>
-  <si>
     <t>URI capture and redirect after logging in</t>
   </si>
   <si>
-    <t>Serializers</t>
-  </si>
-  <si>
     <t>Controllers &amp; APIs</t>
   </si>
   <si>
@@ -424,9 +470,6 @@
     <t>3 ZONES</t>
   </si>
   <si>
-    <t>AGILE</t>
-  </si>
-  <si>
     <t>Testing, Exceptions</t>
   </si>
   <si>
@@ -493,9 +536,6 @@
     <t>Motivational Quotations</t>
   </si>
   <si>
-    <t>Regex, ActiveModel Serializers</t>
-  </si>
-  <si>
     <t>Rails, Web, HTML Verbs</t>
   </si>
   <si>
@@ -517,9 +557,6 @@
     <t>Databases, Migrations</t>
   </si>
   <si>
-    <t>MVP</t>
-  </si>
-  <si>
     <t>Make-your-own API</t>
   </si>
   <si>
@@ -535,14 +572,77 @@
     <t>Health Tracker</t>
   </si>
   <si>
-    <t>Scaffold, Helpers/Partials</t>
+    <t>REST, Scaffold</t>
+  </si>
+  <si>
+    <t>Helpers/Partials, SCSS/Bootstrap</t>
+  </si>
+  <si>
+    <t>JSON, ActiveModel Serializers</t>
+  </si>
+  <si>
+    <t>Regex, Scope</t>
+  </si>
+  <si>
+    <t>SQL, AREL</t>
+  </si>
+  <si>
+    <t>Asset Pipeline</t>
+  </si>
+  <si>
+    <t>Intermediate Rails</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Ex</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>CULTURE</t>
+  </si>
+  <si>
+    <t>Consuming API?</t>
+  </si>
+  <si>
+    <t>Making API?</t>
+  </si>
+  <si>
+    <t>http://www.vikingcodeschool.com/posts/why-learning-to-code-is-so-damn-hard</t>
+  </si>
+  <si>
+    <t>SCARRING w/ AGE</t>
+  </si>
+  <si>
+    <t>AGILE &amp; MVP</t>
+  </si>
+  <si>
+    <t>Gradebook</t>
+  </si>
+  <si>
+    <t>Teacher Rolodex</t>
+  </si>
+  <si>
+    <t>accepts_nested_attributes</t>
+  </si>
+  <si>
+    <t>Session, Authentication</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>Survey Opossum?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -583,6 +683,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -593,13 +700,31 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -611,7 +736,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -649,6 +774,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -670,14 +812,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="37"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="74">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -696,16 +839,25 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -724,16 +876,24 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1062,14 +1222,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomRight" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1081,12 +1241,13 @@
     <col min="6" max="6" width="18.83203125" customWidth="1"/>
     <col min="7" max="7" width="25.1640625" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="3"/>
+    <col min="9" max="12" width="3.5" customWidth="1"/>
+    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,28 +1261,34 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="J1" t="s">
-        <v>152</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>172</v>
+      </c>
+      <c r="M1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" t="s">
+        <v>147</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1129,169 +1296,169 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:15">
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>141</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="G5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>134</v>
+        <v>179</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>19</v>
+      </c>
+      <c r="M10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:15">
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>19</v>
+      </c>
+      <c r="N12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G13" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H13" t="s">
-        <v>155</v>
-      </c>
-      <c r="I13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+        <v>150</v>
+      </c>
+      <c r="M13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1299,97 +1466,110 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:15">
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F16" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="F17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="F18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="C19" t="s">
         <v>7</v>
       </c>
+      <c r="D19" t="s">
+        <v>167</v>
+      </c>
       <c r="F19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>152</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="C23" t="s">
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>153</v>
+      </c>
+      <c r="H23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>166</v>
+      </c>
+      <c r="H24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="C25" t="s">
         <v>7</v>
       </c>
       <c r="D25" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>159</v>
+      </c>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27">
         <v>5</v>
       </c>
@@ -1397,186 +1577,211 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:15">
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E28" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="F28" t="s">
+        <v>178</v>
       </c>
       <c r="H28" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="H29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="H30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="C31" t="s">
         <v>7</v>
       </c>
+      <c r="D31" t="s">
+        <v>165</v>
+      </c>
       <c r="H31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>163</v>
+      </c>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="C34" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="D34" t="s">
+        <v>169</v>
+      </c>
+      <c r="H34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="C35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="D35" t="s">
+        <v>183</v>
+      </c>
+      <c r="H35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="C36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="D36" t="s">
+        <v>184</v>
+      </c>
+      <c r="H36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="C37" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D37" t="s">
+        <v>182</v>
+      </c>
+      <c r="H37" t="s">
+        <v>185</v>
+      </c>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="C40" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:9">
       <c r="C41" t="s">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+    </row>
+    <row r="42" spans="1:9">
       <c r="C42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:9">
       <c r="C43" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="I43" s="5"/>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="C46" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:9">
       <c r="C47" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:9">
       <c r="C48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:14">
       <c r="C49" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="I49" s="5"/>
+    </row>
+    <row r="51" spans="1:14">
       <c r="A51">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:14">
       <c r="C52" t="s">
         <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>26</v>
-      </c>
-      <c r="J52" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+        <v>168</v>
+      </c>
+      <c r="N52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
       <c r="C53" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
       <c r="C54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:14">
       <c r="C55" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
-      <c r="B57" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="B58" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:14">
       <c r="B59" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1602,433 +1807,433 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" t="s">
         <v>99</v>
-      </c>
-      <c r="C43" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Break out old week 5.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -45,7 +45,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Deploy to Heroku</t>
+Data Structure Diagram</t>
         </r>
       </text>
     </comment>
@@ -69,7 +69,55 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+Deploy to Heroku</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mason:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 Existing Codebase</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mason:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TDD</t>
         </r>
       </text>
     </comment>
@@ -78,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="191">
   <si>
     <t>Wk#</t>
   </si>
@@ -548,9 +596,6 @@
     <t>Emp &amp; Dept in Database</t>
   </si>
   <si>
-    <t>Data Diagrams (many)</t>
-  </si>
-  <si>
     <t>Wallet</t>
   </si>
   <si>
@@ -566,9 +611,6 @@
     <t>ActiveRecord, Dev vs. Test</t>
   </si>
   <si>
-    <t>Associations, Validations</t>
-  </si>
-  <si>
     <t>Health Tracker</t>
   </si>
   <si>
@@ -581,15 +623,9 @@
     <t>JSON, ActiveModel Serializers</t>
   </si>
   <si>
-    <t>Regex, Scope</t>
-  </si>
-  <si>
     <t>SQL, AREL</t>
   </si>
   <si>
-    <t>Asset Pipeline</t>
-  </si>
-  <si>
     <t>Intermediate Rails</t>
   </si>
   <si>
@@ -608,9 +644,6 @@
     <t>Consuming API?</t>
   </si>
   <si>
-    <t>Making API?</t>
-  </si>
-  <si>
     <t>http://www.vikingcodeschool.com/posts/why-learning-to-code-is-so-damn-hard</t>
   </si>
   <si>
@@ -635,14 +668,51 @@
     <t>Authorization</t>
   </si>
   <si>
-    <t>Survey Opossum?</t>
+    <t>Associations, Validations, Seeds</t>
+  </si>
+  <si>
+    <t>Address Book Data Str?</t>
+  </si>
+  <si>
+    <t>Regex, Scope, Delegate</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>FRI</t>
+  </si>
+  <si>
+    <t>DATA vs BEHAVIOR</t>
+  </si>
+  <si>
+    <t>Survey Opossum Setup</t>
+  </si>
+  <si>
+    <t>Group project kickoff</t>
+  </si>
+  <si>
+    <t>Survey Opossum</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Asset Pipeline, Workflow Diagrams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -690,6 +760,20 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -713,8 +797,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -724,6 +814,22 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -736,91 +842,106 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="74">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="37"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="37"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="40"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="39"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="38"/>
   </cellXfs>
-  <cellStyles count="74">
+  <cellStyles count="83">
+    <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
+    <cellStyle name="Bad" xfId="38" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -839,24 +960,27 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -876,24 +1000,28 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1223,13 +1351,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H37" sqref="H37"/>
+      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1241,13 +1369,13 @@
     <col min="6" max="6" width="18.83203125" customWidth="1"/>
     <col min="7" max="7" width="25.1640625" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="3.5" customWidth="1"/>
-    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.6640625" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="3"/>
+    <col min="9" max="13" width="3.5" customWidth="1"/>
+    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1273,22 +1401,28 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>171</v>
+        <v>189</v>
       </c>
       <c r="J1" t="s">
-        <v>172</v>
+        <v>167</v>
+      </c>
+      <c r="K1" t="s">
+        <v>168</v>
       </c>
       <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
         <v>138</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1296,7 +1430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="C4" t="s">
         <v>4</v>
       </c>
@@ -1312,11 +1446,11 @@
       <c r="G4" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="C5" t="s">
         <v>5</v>
       </c>
@@ -1332,11 +1466,11 @@
       <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="C6" t="s">
         <v>6</v>
       </c>
@@ -1350,7 +1484,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="C7" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1501,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1375,7 +1509,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="C10" t="s">
         <v>4</v>
       </c>
@@ -1383,7 +1517,7 @@
         <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>141</v>
@@ -1391,11 +1525,11 @@
       <c r="H10" t="s">
         <v>19</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="C11" t="s">
         <v>5</v>
       </c>
@@ -1411,11 +1545,11 @@
       <c r="H11" t="s">
         <v>19</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="C12" t="s">
         <v>6</v>
       </c>
@@ -1431,11 +1565,11 @@
       <c r="H12" t="s">
         <v>19</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="C13" t="s">
         <v>7</v>
       </c>
@@ -1454,11 +1588,12 @@
       <c r="H13" t="s">
         <v>150</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="9"/>
+      <c r="N13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>3</v>
       </c>
@@ -1466,26 +1601,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="H16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
+        <v>181</v>
+      </c>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:16">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F17" t="s">
         <v>124</v>
@@ -1493,30 +1629,34 @@
       <c r="H17" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="I17" s="7"/>
+      <c r="M17" s="9"/>
+    </row>
+    <row r="18" spans="1:16">
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="F18" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="1:16">
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="F19" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="M19" s="9"/>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1524,52 +1664,56 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:16">
       <c r="C22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22" t="s">
         <v>152</v>
       </c>
-      <c r="O22" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="M22" s="9"/>
+      <c r="P22" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="C23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
         <v>153</v>
       </c>
       <c r="H23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
+        <v>171</v>
+      </c>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="1:16">
       <c r="C24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="C25" t="s">
-        <v>7</v>
+        <v>158</v>
+      </c>
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="C25" s="6" t="s">
+        <v>184</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H25" t="s">
-        <v>159</v>
-      </c>
-      <c r="I25" s="5"/>
-    </row>
-    <row r="27" spans="1:15">
+        <v>158</v>
+      </c>
+      <c r="J25" s="5"/>
+      <c r="M25" s="9"/>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27">
         <v>5</v>
       </c>
@@ -1577,7 +1721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:16">
       <c r="C28" t="s">
         <v>4</v>
       </c>
@@ -1588,13 +1732,13 @@
         <v>145</v>
       </c>
       <c r="F28" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H28" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:16">
       <c r="C29" t="s">
         <v>5</v>
       </c>
@@ -1604,177 +1748,206 @@
       <c r="H29" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="M29" s="9"/>
+    </row>
+    <row r="30" spans="1:16">
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
+        <v>156</v>
+      </c>
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" spans="1:16">
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H31" t="s">
-        <v>163</v>
-      </c>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="33" spans="1:9">
+        <v>161</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="5"/>
+      <c r="M31" s="9"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
+        <v>190</v>
+      </c>
+      <c r="F34" t="s">
+        <v>185</v>
+      </c>
+      <c r="H34" t="s">
         <v>169</v>
       </c>
-      <c r="H34" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="M34" s="9"/>
+    </row>
+    <row r="35" spans="1:13">
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H35" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>176</v>
+      </c>
+      <c r="M35" s="9"/>
+    </row>
+    <row r="36" spans="1:13">
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H36" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>175</v>
+      </c>
+      <c r="M36" s="9"/>
+    </row>
+    <row r="37" spans="1:13">
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H37" t="s">
-        <v>185</v>
-      </c>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39">
+        <v>186</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="5"/>
+      <c r="M37" s="9"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="C38" t="s">
+        <v>183</v>
+      </c>
+      <c r="D38" t="s">
+        <v>187</v>
+      </c>
+      <c r="H38" t="s">
+        <v>188</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="M38" s="9"/>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40">
         <v>7</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="C40" t="s">
+    <row r="41" spans="1:13">
+      <c r="C41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
-      <c r="C41" t="s">
+    <row r="42" spans="1:13">
+      <c r="C42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
-      <c r="C42" t="s">
+    <row r="43" spans="1:13">
+      <c r="C43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
-      <c r="C43" t="s">
+    <row r="44" spans="1:13">
+      <c r="C44" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45">
+      <c r="J44" s="5"/>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46">
         <v>8</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
-      <c r="C46" t="s">
+    <row r="47" spans="1:13">
+      <c r="C47" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="C47" t="s">
+      <c r="K47" s="8"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="C48" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:9">
-      <c r="C48" t="s">
+      <c r="K48" s="8"/>
+    </row>
+    <row r="49" spans="1:15">
+      <c r="C49" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
-      <c r="C49" t="s">
+      <c r="K49" s="8"/>
+    </row>
+    <row r="50" spans="1:15">
+      <c r="C50" t="s">
         <v>7</v>
       </c>
-      <c r="I49" s="5"/>
-    </row>
-    <row r="51" spans="1:14">
-      <c r="A51">
+      <c r="J50" s="5"/>
+      <c r="K50" s="8"/>
+    </row>
+    <row r="52" spans="1:15">
+      <c r="A52">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
-      <c r="C52" t="s">
+    <row r="53" spans="1:15">
+      <c r="C53" t="s">
         <v>4</v>
       </c>
-      <c r="D52" t="s">
-        <v>168</v>
-      </c>
-      <c r="N52" t="s">
+      <c r="D53" t="s">
+        <v>165</v>
+      </c>
+      <c r="O53" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
-      <c r="C53" t="s">
+    <row r="54" spans="1:15">
+      <c r="C54" t="s">
         <v>5</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
-      <c r="C54" t="s">
+    <row r="55" spans="1:15">
+      <c r="C55" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:14">
-      <c r="C55" t="s">
+    <row r="56" spans="1:15">
+      <c r="C56" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:14">
-      <c r="B59" t="s">
+    <row r="60" spans="1:15">
+      <c r="B60" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Break out old week 6.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="194">
   <si>
     <t>Wk#</t>
   </si>
@@ -608,9 +608,6 @@
     <t>Dev vs. Prod, Heroku</t>
   </si>
   <si>
-    <t>ActiveRecord, Dev vs. Test</t>
-  </si>
-  <si>
     <t>Health Tracker</t>
   </si>
   <si>
@@ -668,9 +665,6 @@
     <t>Authorization</t>
   </si>
   <si>
-    <t>Associations, Validations, Seeds</t>
-  </si>
-  <si>
     <t>Address Book Data Str?</t>
   </si>
   <si>
@@ -699,6 +693,21 @@
   </si>
   <si>
     <t>Asset Pipeline, Workflow Diagrams</t>
+  </si>
+  <si>
+    <t>Associations, Validations, Seeds/Faker</t>
+  </si>
+  <si>
+    <t>Advanced Rails</t>
+  </si>
+  <si>
+    <t>Efficiency, Metrics</t>
+  </si>
+  <si>
+    <t>Mailer, File Attachments</t>
+  </si>
+  <si>
+    <t>ActiveRecord, Unit Testing/Fixtures</t>
   </si>
 </sst>
 </file>
@@ -842,7 +851,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -884,6 +893,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -939,7 +950,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="39"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="38"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="85">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="Bad" xfId="38" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -981,6 +992,7 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1021,6 +1033,7 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1354,10 +1367,10 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1401,13 +1414,13 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K1" t="s">
         <v>167</v>
-      </c>
-      <c r="K1" t="s">
-        <v>168</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1517,7 +1530,7 @@
         <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>141</v>
@@ -1609,10 +1622,10 @@
         <v>157</v>
       </c>
       <c r="F16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I16" s="7"/>
     </row>
@@ -1621,7 +1634,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="F17" t="s">
         <v>124</v>
@@ -1637,7 +1650,7 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="F18" t="s">
         <v>128</v>
@@ -1649,7 +1662,7 @@
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F19" t="s">
         <v>143</v>
@@ -1673,7 +1686,7 @@
       </c>
       <c r="M22" s="9"/>
       <c r="P22" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1684,7 +1697,7 @@
         <v>153</v>
       </c>
       <c r="H23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M23" s="9"/>
     </row>
@@ -1693,7 +1706,7 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H24" t="s">
         <v>158</v>
@@ -1702,7 +1715,7 @@
     </row>
     <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D25" t="s">
         <v>159</v>
@@ -1732,7 +1745,7 @@
         <v>145</v>
       </c>
       <c r="F28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H28" t="s">
         <v>144</v>
@@ -1755,7 +1768,7 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H30" t="s">
         <v>156</v>
@@ -1767,10 +1780,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="5"/>
@@ -1781,7 +1794,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1789,13 +1802,13 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F34" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M34" s="9"/>
     </row>
@@ -1804,10 +1817,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -1816,10 +1829,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -1828,10 +1841,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="5"/>
@@ -1839,13 +1852,13 @@
     </row>
     <row r="38" spans="1:13">
       <c r="C38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J38" s="5"/>
       <c r="M38" s="9"/>
@@ -1884,19 +1897,25 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="C47" t="s">
         <v>4</v>
       </c>
+      <c r="D47" t="s">
+        <v>164</v>
+      </c>
       <c r="K47" s="8"/>
     </row>
     <row r="48" spans="1:13">
       <c r="C48" t="s">
         <v>5</v>
       </c>
+      <c r="D48" t="s">
+        <v>192</v>
+      </c>
       <c r="K48" s="8"/>
     </row>
     <row r="49" spans="1:15">
@@ -1916,13 +1935,16 @@
       <c r="A52">
         <v>9</v>
       </c>
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="53" spans="1:15">
       <c r="C53" t="s">
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="O53" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Break out old week 7.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="202">
   <si>
     <t>Wk#</t>
   </si>
@@ -708,6 +708,30 @@
   </si>
   <si>
     <t>ActiveRecord, Unit Testing/Fixtures</t>
+  </si>
+  <si>
+    <t>Add JavaScript</t>
+  </si>
+  <si>
+    <t>Add jQuery</t>
+  </si>
+  <si>
+    <t>jQuery</t>
+  </si>
+  <si>
+    <t>AJAX</t>
+  </si>
+  <si>
+    <t>Auction Site</t>
+  </si>
+  <si>
+    <t>Todo List</t>
+  </si>
+  <si>
+    <t>JavaScript in Depth</t>
+  </si>
+  <si>
+    <t>AUTON/MAST/PURP</t>
   </si>
 </sst>
 </file>
@@ -851,7 +875,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -893,6 +917,10 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -950,7 +978,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="39"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="38"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="89">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="Bad" xfId="38" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -993,6 +1021,8 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1034,6 +1064,8 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1367,10 +1399,10 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1875,21 +1907,48 @@
       <c r="C41" t="s">
         <v>4</v>
       </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" t="s">
+        <v>201</v>
+      </c>
+      <c r="H41" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="42" spans="1:13">
       <c r="C42" t="s">
         <v>5</v>
       </c>
+      <c r="D42" t="s">
+        <v>196</v>
+      </c>
+      <c r="H42" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="43" spans="1:13">
       <c r="C43" t="s">
         <v>6</v>
       </c>
+      <c r="D43" t="s">
+        <v>197</v>
+      </c>
+      <c r="H43" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="44" spans="1:13">
       <c r="C44" t="s">
         <v>7</v>
       </c>
+      <c r="D44" t="s">
+        <v>200</v>
+      </c>
+      <c r="H44" t="s">
+        <v>199</v>
+      </c>
       <c r="J44" s="5"/>
     </row>
     <row r="46" spans="1:13">
@@ -1907,7 +1966,6 @@
       <c r="D47" t="s">
         <v>164</v>
       </c>
-      <c r="K47" s="8"/>
     </row>
     <row r="48" spans="1:13">
       <c r="C48" t="s">
@@ -1916,20 +1974,17 @@
       <c r="D48" t="s">
         <v>192</v>
       </c>
-      <c r="K48" s="8"/>
     </row>
     <row r="49" spans="1:15">
       <c r="C49" t="s">
         <v>6</v>
       </c>
-      <c r="K49" s="8"/>
     </row>
     <row r="50" spans="1:15">
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="J50" s="5"/>
-      <c r="K50" s="8"/>
     </row>
     <row r="52" spans="1:15">
       <c r="A52">
@@ -1946,9 +2001,7 @@
       <c r="D53" t="s">
         <v>191</v>
       </c>
-      <c r="O53" t="s">
-        <v>23</v>
-      </c>
+      <c r="K53" s="8"/>
     </row>
     <row r="54" spans="1:15">
       <c r="C54" t="s">
@@ -1957,16 +2010,22 @@
       <c r="D54" t="s">
         <v>22</v>
       </c>
+      <c r="K54" s="8"/>
+      <c r="O54" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="55" spans="1:15">
       <c r="C55" t="s">
         <v>6</v>
       </c>
+      <c r="K55" s="8"/>
     </row>
     <row r="56" spans="1:15">
       <c r="C56" t="s">
         <v>7</v>
       </c>
+      <c r="K56" s="8"/>
     </row>
     <row r="60" spans="1:15">
       <c r="B60" t="s">

</xml_diff>

<commit_message>
Break out old week 8.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="205">
   <si>
     <t>Wk#</t>
   </si>
@@ -170,6 +170,9 @@
     <t>Know Thy Error Message, know the class of things stored in your variables</t>
   </si>
   <si>
+    <t>APIs</t>
+  </si>
+  <si>
     <t>Legacy Code</t>
   </si>
   <si>
@@ -587,9 +590,6 @@
     <t>Rails, Web, HTML Verbs</t>
   </si>
   <si>
-    <t>Router, Controllers</t>
-  </si>
-  <si>
     <t>HTML Forms, ERB</t>
   </si>
   <si>
@@ -605,9 +605,6 @@
     <t>Make-your-own API</t>
   </si>
   <si>
-    <t>Dev vs. Prod, Heroku</t>
-  </si>
-  <si>
     <t>Health Tracker</t>
   </si>
   <si>
@@ -638,9 +635,6 @@
     <t>CULTURE</t>
   </si>
   <si>
-    <t>Consuming API?</t>
-  </si>
-  <si>
     <t>http://www.vikingcodeschool.com/posts/why-learning-to-code-is-so-damn-hard</t>
   </si>
   <si>
@@ -668,9 +662,6 @@
     <t>Address Book Data Str?</t>
   </si>
   <si>
-    <t>Regex, Scope, Delegate</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -695,9 +686,6 @@
     <t>Asset Pipeline, Workflow Diagrams</t>
   </si>
   <si>
-    <t>Associations, Validations, Seeds/Faker</t>
-  </si>
-  <si>
     <t>Advanced Rails</t>
   </si>
   <si>
@@ -707,18 +695,12 @@
     <t>Mailer, File Attachments</t>
   </si>
   <si>
-    <t>ActiveRecord, Unit Testing/Fixtures</t>
-  </si>
-  <si>
     <t>Add JavaScript</t>
   </si>
   <si>
     <t>Add jQuery</t>
   </si>
   <si>
-    <t>jQuery</t>
-  </si>
-  <si>
     <t>AJAX</t>
   </si>
   <si>
@@ -732,13 +714,40 @@
   </si>
   <si>
     <t>AUTON/MAST/PURP</t>
+  </si>
+  <si>
+    <t>jQuery, UJ</t>
+  </si>
+  <si>
+    <t>TECHNICAL DEBT</t>
+  </si>
+  <si>
+    <t>Consume API</t>
+  </si>
+  <si>
+    <t>Associations, Validations, Seeds/Faker, Scope, Delegate</t>
+  </si>
+  <si>
+    <t>ActiveRecord, Unit Testing/Fixtures, Efficiency</t>
+  </si>
+  <si>
+    <t>Router, Controllers, Regex</t>
+  </si>
+  <si>
+    <t>API Security, oAuth</t>
+  </si>
+  <si>
+    <t>Dev vs. Prod, Heroku, Servers</t>
+  </si>
+  <si>
+    <t>Life as a Dev, Ruby on Not Rails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -836,6 +845,11 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -875,7 +889,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="89">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -965,8 +979,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -977,8 +993,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="40"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="39"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="38"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="89">
+  <cellStyles count="91">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="Bad" xfId="38" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1023,6 +1040,7 @@
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1066,6 +1084,7 @@
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1399,10 +1418,10 @@
   <dimension ref="A1:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1434,37 +1453,37 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" t="s">
         <v>122</v>
-      </c>
-      <c r="G1" t="s">
-        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" t="s">
         <v>166</v>
-      </c>
-      <c r="K1" t="s">
-        <v>167</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="O1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1480,19 +1499,19 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="N4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1500,19 +1519,19 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1520,13 +1539,13 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1534,16 +1553,16 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H7" t="s">
         <v>141</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H7" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1551,7 +1570,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1559,19 +1578,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1579,16 +1598,16 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>13</v>
@@ -1599,19 +1618,19 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1619,23 +1638,23 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" t="s">
         <v>133</v>
       </c>
-      <c r="G13" t="s">
-        <v>132</v>
-      </c>
       <c r="H13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1654,10 +1673,10 @@
         <v>157</v>
       </c>
       <c r="F16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I16" s="7"/>
     </row>
@@ -1666,10 +1685,10 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="F17" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H17" t="s">
         <v>155</v>
@@ -1682,10 +1701,10 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="F18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M18" s="9"/>
     </row>
@@ -1693,11 +1712,14 @@
       <c r="C19" t="s">
         <v>7</v>
       </c>
-      <c r="D19" t="s">
-        <v>180</v>
+      <c r="D19" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>144</v>
+      </c>
+      <c r="H19" t="s">
+        <v>198</v>
       </c>
       <c r="M19" s="9"/>
     </row>
@@ -1706,7 +1728,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1714,11 +1736,11 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M22" s="9"/>
       <c r="P22" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1726,10 +1748,7 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
-      </c>
-      <c r="H23" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="M23" s="9"/>
     </row>
@@ -1738,7 +1757,7 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H24" t="s">
         <v>158</v>
@@ -1747,10 +1766,10 @@
     </row>
     <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>203</v>
       </c>
       <c r="H25" t="s">
         <v>158</v>
@@ -1771,16 +1790,16 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E28" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" t="s">
+        <v>170</v>
+      </c>
+      <c r="H28" t="s">
         <v>145</v>
-      </c>
-      <c r="F28" t="s">
-        <v>172</v>
-      </c>
-      <c r="H28" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1791,7 +1810,7 @@
         <v>154</v>
       </c>
       <c r="H29" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="M29" s="9"/>
     </row>
@@ -1800,7 +1819,7 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H30" t="s">
         <v>156</v>
@@ -1812,10 +1831,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="5"/>
@@ -1826,7 +1845,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1834,13 +1853,13 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F34" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M34" s="9"/>
     </row>
@@ -1849,10 +1868,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H35" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -1861,10 +1880,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -1873,10 +1892,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H37" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="5"/>
@@ -1884,13 +1903,13 @@
     </row>
     <row r="38" spans="1:13">
       <c r="C38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D38" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H38" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J38" s="5"/>
       <c r="M38" s="9"/>
@@ -1911,10 +1930,10 @@
         <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="H41" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -1925,7 +1944,7 @@
         <v>196</v>
       </c>
       <c r="H42" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -1933,10 +1952,10 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H43" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -1944,10 +1963,10 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="H44" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J44" s="5"/>
     </row>
@@ -1956,7 +1975,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -1964,7 +1983,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>164</v>
+        <v>163</v>
+      </c>
+      <c r="F47" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -1972,18 +1994,24 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:15">
       <c r="C49" t="s">
         <v>6</v>
       </c>
+      <c r="D49" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="50" spans="1:15">
       <c r="C50" t="s">
         <v>7</v>
       </c>
+      <c r="D50" t="s">
+        <v>204</v>
+      </c>
       <c r="J50" s="5"/>
     </row>
     <row r="52" spans="1:15">
@@ -1991,7 +2019,7 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -1999,7 +2027,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2008,11 +2036,11 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K54" s="8"/>
       <c r="O54" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:15">
@@ -2029,7 +2057,7 @@
     </row>
     <row r="60" spans="1:15">
       <c r="B60" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2061,433 +2089,433 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
         <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
         <v>54</v>
-      </c>
-      <c r="B14" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" t="s">
         <v>66</v>
-      </c>
-      <c r="C18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" t="s">
         <v>69</v>
       </c>
-      <c r="B19" t="s">
-        <v>68</v>
-      </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
         <v>77</v>
       </c>
-      <c r="B28" t="s">
-        <v>76</v>
-      </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s">
         <v>81</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>80</v>
-      </c>
-      <c r="C34" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Break out old week 9.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -45,7 +45,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Data Structure Diagram</t>
+Blue: Data Structure Diagram
+Purple: Workflow Diagram</t>
         </r>
       </text>
     </comment>
@@ -97,6 +98,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mason:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Create Estimate</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="M1" authorId="0">
       <text>
         <r>
@@ -126,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="212">
   <si>
     <t>Wk#</t>
   </si>
@@ -176,9 +201,6 @@
     <t>Legacy Code</t>
   </si>
   <si>
-    <t>URI capture and redirect after logging in</t>
-  </si>
-  <si>
     <t>Controllers &amp; APIs</t>
   </si>
   <si>
@@ -617,9 +639,6 @@
     <t>JSON, ActiveModel Serializers</t>
   </si>
   <si>
-    <t>SQL, AREL</t>
-  </si>
-  <si>
     <t>Intermediate Rails</t>
   </si>
   <si>
@@ -647,9 +666,6 @@
     <t>Gradebook</t>
   </si>
   <si>
-    <t>Teacher Rolodex</t>
-  </si>
-  <si>
     <t>accepts_nested_attributes</t>
   </si>
   <si>
@@ -689,12 +705,6 @@
     <t>Advanced Rails</t>
   </si>
   <si>
-    <t>Efficiency, Metrics</t>
-  </si>
-  <si>
-    <t>Mailer, File Attachments</t>
-  </si>
-  <si>
     <t>Add JavaScript</t>
   </si>
   <si>
@@ -740,7 +750,43 @@
     <t>Dev vs. Prod, Heroku, Servers</t>
   </si>
   <si>
-    <t>Life as a Dev, Ruby on Not Rails</t>
+    <t>Runtime and Metrics</t>
+  </si>
+  <si>
+    <t>Memory and Metrics</t>
+  </si>
+  <si>
+    <t>SQL, AREL, Indices</t>
+  </si>
+  <si>
+    <t>Database Optimizations</t>
+  </si>
+  <si>
+    <t>Mailer, Delayed Job</t>
+  </si>
+  <si>
+    <t>File Uploads</t>
+  </si>
+  <si>
+    <t>Delayed Mailer</t>
+  </si>
+  <si>
+    <t>Reports on S3</t>
+  </si>
+  <si>
+    <t>Ruby on Not Rails</t>
+  </si>
+  <si>
+    <t>LIFE AS A DEV</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Teacherbook</t>
+  </si>
+  <si>
+    <t>Modify existing?</t>
   </si>
 </sst>
 </file>
@@ -851,7 +897,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -879,6 +925,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -889,7 +947,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -931,6 +989,48 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -982,7 +1082,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -994,9 +1094,13 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="39"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="38"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="133">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
+    <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
+    <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
     <cellStyle name="Bad" xfId="38" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1016,7 +1120,6 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
@@ -1041,6 +1144,27 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1060,7 +1184,6 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
@@ -1085,6 +1208,27 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1415,13 +1559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D17" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1453,37 +1595,40 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K1" t="s">
-        <v>166</v>
+        <v>164</v>
+      </c>
+      <c r="L1" t="s">
+        <v>209</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1499,19 +1644,19 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1519,19 +1664,19 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1539,13 +1684,13 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1553,16 +1698,16 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1570,7 +1715,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1578,19 +1723,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
-      </c>
-      <c r="F10" t="s">
-        <v>171</v>
+        <v>130</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1598,16 +1743,16 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>169</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>13</v>
@@ -1618,19 +1763,20 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="L12" s="12"/>
       <c r="O12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1638,23 +1784,23 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" t="s">
         <v>150</v>
-      </c>
-      <c r="E13" t="s">
-        <v>143</v>
-      </c>
-      <c r="F13" t="s">
-        <v>134</v>
-      </c>
-      <c r="G13" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13" t="s">
-        <v>151</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1670,13 +1816,10 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
-      </c>
-      <c r="F16" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="H16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I16" s="7"/>
     </row>
@@ -1685,13 +1828,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F17" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="H17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I17" s="7"/>
       <c r="M17" s="9"/>
@@ -1701,11 +1844,15 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F18" t="s">
-        <v>129</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="H18" t="s">
+        <v>211</v>
+      </c>
+      <c r="K18" s="8"/>
       <c r="M18" s="9"/>
     </row>
     <row r="19" spans="1:16">
@@ -1716,10 +1863,10 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H19" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="M19" s="9"/>
     </row>
@@ -1728,7 +1875,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1736,11 +1883,11 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M22" s="9"/>
       <c r="P22" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1748,7 +1895,10 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>201</v>
+        <v>196</v>
+      </c>
+      <c r="F23" t="s">
+        <v>168</v>
       </c>
       <c r="M23" s="9"/>
     </row>
@@ -1757,22 +1907,25 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>162</v>
+        <v>161</v>
+      </c>
+      <c r="F24" t="s">
+        <v>128</v>
       </c>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D25" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J25" s="5"/>
       <c r="M25" s="9"/>
@@ -1790,16 +1943,13 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E28" t="s">
-        <v>146</v>
-      </c>
-      <c r="F28" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="H28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1807,11 +1957,15 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>153</v>
+      </c>
+      <c r="F29" t="s">
+        <v>177</v>
       </c>
       <c r="H29" t="s">
-        <v>152</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="I29" s="11"/>
       <c r="M29" s="9"/>
     </row>
     <row r="30" spans="1:16">
@@ -1819,11 +1973,12 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H30" t="s">
-        <v>156</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="I30" s="11"/>
       <c r="M30" s="9"/>
     </row>
     <row r="31" spans="1:16">
@@ -1831,10 +1986,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="5"/>
@@ -1845,7 +2000,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -1853,13 +2008,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>185</v>
-      </c>
-      <c r="F34" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M34" s="9"/>
     </row>
@@ -1868,10 +2020,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H35" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -1880,10 +2032,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H36" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -1892,10 +2044,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H37" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="5"/>
@@ -1903,13 +2055,13 @@
     </row>
     <row r="38" spans="1:13">
       <c r="C38" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D38" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H38" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J38" s="5"/>
       <c r="M38" s="9"/>
@@ -1929,11 +2081,8 @@
       <c r="D41" t="s">
         <v>11</v>
       </c>
-      <c r="F41" t="s">
-        <v>195</v>
-      </c>
       <c r="H41" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -1941,10 +2090,13 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>196</v>
+        <v>191</v>
+      </c>
+      <c r="F42" t="s">
+        <v>190</v>
       </c>
       <c r="H42" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -1952,10 +2104,10 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H43" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -1963,10 +2115,10 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H44" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="J44" s="5"/>
     </row>
@@ -1975,7 +2127,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -1983,10 +2135,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>163</v>
-      </c>
-      <c r="F47" t="s">
-        <v>197</v>
+        <v>201</v>
+      </c>
+      <c r="H47" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -1994,7 +2146,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>188</v>
+        <v>203</v>
+      </c>
+      <c r="F48" t="s">
+        <v>192</v>
+      </c>
+      <c r="H48" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -2002,7 +2160,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>204</v>
+      </c>
+      <c r="H49" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -2010,7 +2171,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2027,7 +2188,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2036,28 +2197,34 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>23</v>
+        <v>200</v>
+      </c>
+      <c r="F54" t="s">
+        <v>208</v>
       </c>
       <c r="K54" s="8"/>
-      <c r="O54" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="55" spans="1:15">
       <c r="C55" t="s">
         <v>6</v>
       </c>
+      <c r="D55" t="s">
+        <v>22</v>
+      </c>
       <c r="K55" s="8"/>
     </row>
     <row r="56" spans="1:15">
       <c r="C56" t="s">
         <v>7</v>
       </c>
-      <c r="K56" s="8"/>
-    </row>
-    <row r="60" spans="1:15">
-      <c r="B60" t="s">
-        <v>16</v>
+      <c r="D56" t="s">
+        <v>207</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2089,433 +2256,433 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
         <v>76</v>
       </c>
-      <c r="B26" t="s">
-        <v>77</v>
-      </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
         <v>109</v>
-      </c>
-      <c r="B29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
         <v>112</v>
-      </c>
-      <c r="B31" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" t="s">
         <v>105</v>
-      </c>
-      <c r="B33" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
         <v>101</v>
-      </c>
-      <c r="B35" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
         <v>114</v>
-      </c>
-      <c r="B36" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
         <v>84</v>
-      </c>
-      <c r="B38" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" t="s">
         <v>92</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>93</v>
-      </c>
-      <c r="C41" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" t="s">
         <v>95</v>
       </c>
-      <c r="B43" t="s">
-        <v>96</v>
-      </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
         <v>97</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>98</v>
-      </c>
-      <c r="C44" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" t="s">
         <v>33</v>
-      </c>
-      <c r="B55" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" t="s">
         <v>35</v>
-      </c>
-      <c r="B56" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begin work on migrating information from old weeks to new weeks.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -672,9 +672,6 @@
     <t>Session, Authentication</t>
   </si>
   <si>
-    <t>Authorization</t>
-  </si>
-  <si>
     <t>Address Book Data Str?</t>
   </si>
   <si>
@@ -702,6 +699,9 @@
     <t>Asset Pipeline, Workflow Diagrams</t>
   </si>
   <si>
+    <t>Associations, Validations, Seeds/Faker</t>
+  </si>
+  <si>
     <t>Advanced Rails</t>
   </si>
   <si>
@@ -735,9 +735,6 @@
     <t>Consume API</t>
   </si>
   <si>
-    <t>Associations, Validations, Seeds/Faker, Scope, Delegate</t>
-  </si>
-  <si>
     <t>ActiveRecord, Unit Testing/Fixtures, Efficiency</t>
   </si>
   <si>
@@ -787,6 +784,9 @@
   </si>
   <si>
     <t>Modify existing?</t>
+  </si>
+  <si>
+    <t>Authorization, Scope, Delegate</t>
   </si>
 </sst>
 </file>
@@ -1562,8 +1562,8 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1607,7 +1607,7 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J1" t="s">
         <v>163</v>
@@ -1616,7 +1616,7 @@
         <v>164</v>
       </c>
       <c r="L1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1819,7 +1819,7 @@
         <v>156</v>
       </c>
       <c r="H16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I16" s="7"/>
     </row>
@@ -1828,7 +1828,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F17" t="s">
         <v>166</v>
@@ -1844,13 +1844,13 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="F18" t="s">
         <v>124</v>
       </c>
       <c r="H18" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
@@ -1895,7 +1895,7 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F23" t="s">
         <v>168</v>
@@ -1919,10 +1919,10 @@
     </row>
     <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H25" t="s">
         <v>157</v>
@@ -1960,7 +1960,7 @@
         <v>153</v>
       </c>
       <c r="F29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H29" t="s">
         <v>151</v>
@@ -2008,7 +2008,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H34" t="s">
         <v>165</v>
@@ -2023,7 +2023,7 @@
         <v>172</v>
       </c>
       <c r="H35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2032,7 +2032,7 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="H36" t="s">
         <v>170</v>
@@ -2047,7 +2047,7 @@
         <v>171</v>
       </c>
       <c r="H37" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="5"/>
@@ -2055,13 +2055,13 @@
     </row>
     <row r="38" spans="1:13">
       <c r="C38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D38" t="s">
+        <v>178</v>
+      </c>
+      <c r="H38" t="s">
         <v>179</v>
-      </c>
-      <c r="H38" t="s">
-        <v>180</v>
       </c>
       <c r="J38" s="5"/>
       <c r="M38" s="9"/>
@@ -2135,10 +2135,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>200</v>
+      </c>
+      <c r="H47" t="s">
         <v>201</v>
-      </c>
-      <c r="H47" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2146,13 +2146,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F48" t="s">
         <v>192</v>
       </c>
       <c r="H48" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -2160,10 +2160,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -2171,7 +2171,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2188,7 +2188,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2197,10 +2197,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2218,7 +2218,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
Create week 4 skeleton.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="213">
   <si>
     <t>Wk#</t>
   </si>
@@ -195,15 +195,15 @@
     <t>Know Thy Error Message, know the class of things stored in your variables</t>
   </si>
   <si>
-    <t>APIs</t>
-  </si>
-  <si>
     <t>Legacy Code</t>
   </si>
   <si>
     <t>Controllers &amp; APIs</t>
   </si>
   <si>
+    <t>ActiveModel Serializers</t>
+  </si>
+  <si>
     <t>PB&amp;J</t>
   </si>
   <si>
@@ -612,6 +612,9 @@
     <t>Rails, Web, HTML Verbs</t>
   </si>
   <si>
+    <t>Router, Controllers</t>
+  </si>
+  <si>
     <t>HTML Forms, ERB</t>
   </si>
   <si>
@@ -636,9 +639,6 @@
     <t>Helpers/Partials, SCSS/Bootstrap</t>
   </si>
   <si>
-    <t>JSON, ActiveModel Serializers</t>
-  </si>
-  <si>
     <t>Intermediate Rails</t>
   </si>
   <si>
@@ -738,9 +738,6 @@
     <t>ActiveRecord, Unit Testing/Fixtures, Efficiency</t>
   </si>
   <si>
-    <t>Router, Controllers, Regex</t>
-  </si>
-  <si>
     <t>API Security, oAuth</t>
   </si>
   <si>
@@ -787,6 +784,12 @@
   </si>
   <si>
     <t>Authorization, Scope, Delegate</t>
+  </si>
+  <si>
+    <t>Consume API, display HTML</t>
+  </si>
+  <si>
+    <t>APIs, Regex, JSON</t>
   </si>
 </sst>
 </file>
@@ -1562,8 +1565,8 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1616,7 +1619,7 @@
         <v>164</v>
       </c>
       <c r="L1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1816,7 +1819,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H16" t="s">
         <v>173</v>
@@ -1834,7 +1837,7 @@
         <v>166</v>
       </c>
       <c r="H17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I17" s="7"/>
       <c r="M17" s="9"/>
@@ -1850,7 +1853,7 @@
         <v>124</v>
       </c>
       <c r="H18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
@@ -1860,7 +1863,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>14</v>
+        <v>212</v>
       </c>
       <c r="F19" t="s">
         <v>143</v>
@@ -1875,7 +1878,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1895,10 +1898,13 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="F23" t="s">
         <v>168</v>
+      </c>
+      <c r="H23" t="s">
+        <v>211</v>
       </c>
       <c r="M23" s="9"/>
     </row>
@@ -1907,13 +1913,13 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
         <v>128</v>
       </c>
       <c r="H24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="M24" s="9"/>
     </row>
@@ -1922,10 +1928,10 @@
         <v>175</v>
       </c>
       <c r="D25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H25" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="J25" s="5"/>
       <c r="M25" s="9"/>
@@ -1957,7 +1963,7 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F29" t="s">
         <v>176</v>
@@ -1973,10 +1979,10 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I30" s="11"/>
       <c r="M30" s="9"/>
@@ -1986,10 +1992,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="5"/>
@@ -2023,7 +2029,7 @@
         <v>172</v>
       </c>
       <c r="H35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2032,7 +2038,7 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H36" t="s">
         <v>170</v>
@@ -2135,10 +2141,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>199</v>
+      </c>
+      <c r="H47" t="s">
         <v>200</v>
-      </c>
-      <c r="H47" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2146,13 +2152,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F48" t="s">
         <v>192</v>
       </c>
       <c r="H48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -2160,10 +2166,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -2171,7 +2177,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2180,7 +2186,7 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -2188,7 +2194,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2197,10 +2203,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F54" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2218,7 +2224,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
Attempt to place 'recreate github profile' assignment.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="214">
   <si>
     <t>Wk#</t>
   </si>
@@ -732,9 +732,6 @@
     <t>TECHNICAL DEBT</t>
   </si>
   <si>
-    <t>Consume API</t>
-  </si>
-  <si>
     <t>ActiveRecord, Unit Testing/Fixtures, Efficiency</t>
   </si>
   <si>
@@ -790,6 +787,12 @@
   </si>
   <si>
     <t>APIs, Regex, JSON</t>
+  </si>
+  <si>
+    <t>Consume Github API?</t>
+  </si>
+  <si>
+    <t>Consume Weather API?</t>
   </si>
 </sst>
 </file>
@@ -1566,7 +1569,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1619,7 +1622,7 @@
         <v>164</v>
       </c>
       <c r="L1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1831,7 +1834,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F17" t="s">
         <v>166</v>
@@ -1853,7 +1856,7 @@
         <v>124</v>
       </c>
       <c r="H18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
@@ -1863,13 +1866,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F19" t="s">
         <v>143</v>
       </c>
       <c r="H19" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="M19" s="9"/>
     </row>
@@ -1888,6 +1891,9 @@
       <c r="D22" t="s">
         <v>152</v>
       </c>
+      <c r="H22" t="s">
+        <v>212</v>
+      </c>
       <c r="M22" s="9"/>
       <c r="P22" s="3" t="s">
         <v>167</v>
@@ -1904,7 +1910,7 @@
         <v>168</v>
       </c>
       <c r="H23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M23" s="9"/>
     </row>
@@ -1928,7 +1934,7 @@
         <v>175</v>
       </c>
       <c r="D25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H25" t="s">
         <v>158</v>
@@ -2029,7 +2035,7 @@
         <v>172</v>
       </c>
       <c r="H35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2038,7 +2044,7 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H36" t="s">
         <v>170</v>
@@ -2141,10 +2147,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>198</v>
+      </c>
+      <c r="H47" t="s">
         <v>199</v>
-      </c>
-      <c r="H47" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2152,13 +2158,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F48" t="s">
         <v>192</v>
       </c>
       <c r="H48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -2166,10 +2172,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -2177,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2194,7 +2200,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2203,10 +2209,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F54" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2224,7 +2230,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
Begin moving ruby challenges.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27040" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curriculum" sheetId="1" r:id="rId1"/>
@@ -1569,7 +1569,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Distribute old week 8 content.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21120" tabRatio="500"/>
+    <workbookView xWindow="4800" yWindow="21600" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curriculum" sheetId="1" r:id="rId1"/>
@@ -606,9 +606,6 @@
     <t>Employees and Depts?</t>
   </si>
   <si>
-    <t>Motivational Quotations</t>
-  </si>
-  <si>
     <t>Rails, Web, HTML Verbs</t>
   </si>
   <si>
@@ -783,9 +780,6 @@
     <t>Authorization, Scope, Delegate</t>
   </si>
   <si>
-    <t>Consume API, display HTML</t>
-  </si>
-  <si>
     <t>APIs, Regex, JSON</t>
   </si>
   <si>
@@ -793,6 +787,12 @@
   </si>
   <si>
     <t>Consume Weather API?</t>
+  </si>
+  <si>
+    <t>Create Voting API</t>
+  </si>
+  <si>
+    <t>Recreate Github Profile</t>
   </si>
 </sst>
 </file>
@@ -1568,8 +1568,8 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O31" sqref="O31"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1613,16 +1613,16 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" t="s">
         <v>163</v>
       </c>
-      <c r="K1" t="s">
-        <v>164</v>
-      </c>
       <c r="L1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -1752,7 +1752,7 @@
         <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>141</v>
@@ -1822,10 +1822,10 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I16" s="7"/>
     </row>
@@ -1834,13 +1834,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I17" s="7"/>
       <c r="M17" s="9"/>
@@ -1850,13 +1850,13 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F18" t="s">
         <v>124</v>
       </c>
       <c r="H18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
@@ -1866,13 +1866,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F19" t="s">
         <v>143</v>
       </c>
       <c r="H19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M19" s="9"/>
     </row>
@@ -1889,14 +1889,14 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M22" s="9"/>
       <c r="P22" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1904,13 +1904,13 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="M23" s="9"/>
     </row>
@@ -1925,19 +1925,19 @@
         <v>128</v>
       </c>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J25" s="5"/>
       <c r="M25" s="9"/>
@@ -1969,13 +1969,13 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H29" t="s">
-        <v>151</v>
+        <v>213</v>
       </c>
       <c r="I29" s="11"/>
       <c r="M29" s="9"/>
@@ -1985,10 +1985,10 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I30" s="11"/>
       <c r="M30" s="9"/>
@@ -1998,10 +1998,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="5"/>
@@ -2012,7 +2012,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -2020,10 +2020,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M34" s="9"/>
     </row>
@@ -2032,10 +2032,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2044,10 +2044,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -2056,10 +2056,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="5"/>
@@ -2067,13 +2067,13 @@
     </row>
     <row r="38" spans="1:13">
       <c r="C38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D38" t="s">
+        <v>177</v>
+      </c>
+      <c r="H38" t="s">
         <v>178</v>
-      </c>
-      <c r="H38" t="s">
-        <v>179</v>
       </c>
       <c r="J38" s="5"/>
       <c r="M38" s="9"/>
@@ -2094,7 +2094,7 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2102,13 +2102,13 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F42" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2116,10 +2116,10 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
+        <v>185</v>
+      </c>
+      <c r="H43" t="s">
         <v>186</v>
-      </c>
-      <c r="H43" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2127,10 +2127,10 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J44" s="5"/>
     </row>
@@ -2139,7 +2139,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2147,10 +2147,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>197</v>
+      </c>
+      <c r="H47" t="s">
         <v>198</v>
-      </c>
-      <c r="H47" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2158,13 +2158,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -2172,10 +2172,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -2183,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J50" s="5"/>
     </row>
@@ -2200,7 +2200,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2209,10 +2209,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2230,7 +2230,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>141</v>

</xml_diff>

<commit_message>
Finish Week 1 Day 2.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -45,8 +45,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Blue: Data Structure Diagram
-Purple: Workflow Diagram</t>
+Pair Programming</t>
         </r>
       </text>
     </comment>
@@ -70,7 +69,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Deploy to Heroku</t>
+Blue: Data Structure Diagram
+Purple: Workflow Diagram</t>
         </r>
       </text>
     </comment>
@@ -94,7 +94,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Existing Codebase</t>
+Deploy to Heroku</t>
         </r>
       </text>
     </comment>
@@ -118,11 +118,35 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
+Existing Codebase</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mason:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 Create Estimate</t>
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="215">
   <si>
     <t>Wk#</t>
   </si>
@@ -213,12 +237,6 @@
     <t>Battleship</t>
   </si>
   <si>
-    <t>Methods</t>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
     <t>Skinny Models</t>
   </si>
   <si>
@@ -510,15 +528,9 @@
     <t>Nested Joins</t>
   </si>
   <si>
-    <t>init, clone, add, commit, push</t>
-  </si>
-  <si>
     <t>Classes</t>
   </si>
   <si>
-    <t>Git</t>
-  </si>
-  <si>
     <t>Human Learning</t>
   </si>
   <si>
@@ -528,9 +540,6 @@
     <t>Googling</t>
   </si>
   <si>
-    <t>Enumerables</t>
-  </si>
-  <si>
     <t>Enumerables, Inheritance</t>
   </si>
   <si>
@@ -549,9 +558,6 @@
     <t>Composition, Modules</t>
   </si>
   <si>
-    <t>branch, pull</t>
-  </si>
-  <si>
     <t>Pair Programming</t>
   </si>
   <si>
@@ -567,12 +573,6 @@
     <t>Hashes, Nested Data Structures</t>
   </si>
   <si>
-    <t>Assignment leads to</t>
-  </si>
-  <si>
-    <t>next, break, return, exit</t>
-  </si>
-  <si>
     <t>Currency Converter</t>
   </si>
   <si>
@@ -591,9 +591,6 @@
     <t>Personal Site</t>
   </si>
   <si>
-    <t>Motivating Ex.</t>
-  </si>
-  <si>
     <t>Reading/Listening</t>
   </si>
   <si>
@@ -793,6 +790,36 @@
   </si>
   <si>
     <t>Recreate Github Profile</t>
+  </si>
+  <si>
+    <t>Markdown, READMEs</t>
+  </si>
+  <si>
+    <t>Input Statistics</t>
+  </si>
+  <si>
+    <t>12 Days of Christmas</t>
+  </si>
+  <si>
+    <t>Git/Github</t>
+  </si>
+  <si>
+    <t>init, add, commit, push</t>
+  </si>
+  <si>
+    <t>fork, clone</t>
+  </si>
+  <si>
+    <t>Problem of the Day</t>
+  </si>
+  <si>
+    <t>branch, pull, merge</t>
+  </si>
+  <si>
+    <t>Try to solve before being taught</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -953,7 +980,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -997,6 +1024,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1103,7 +1134,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="137">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1171,6 +1202,8 @@
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1235,6 +1268,8 @@
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1568,8 +1603,8 @@
   <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1577,12 +1612,11 @@
     <col min="1" max="1" width="5.1640625" customWidth="1"/>
     <col min="3" max="3" width="4.5" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.1640625" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="3.5" customWidth="1"/>
-    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="3.5" customWidth="1"/>
     <col min="15" max="15" width="23.6640625" customWidth="1"/>
     <col min="16" max="16" width="10.83203125" style="3"/>
   </cols>
@@ -1601,40 +1635,40 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>211</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G1" t="s">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
       <c r="J1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="K1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="L1" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
       <c r="M1" t="s">
+        <v>196</v>
+      </c>
+      <c r="N1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>138</v>
       </c>
-      <c r="O1" t="s">
-        <v>147</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1650,19 +1684,22 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="N4" t="s">
-        <v>20</v>
+        <v>133</v>
+      </c>
+      <c r="H4" t="s">
+        <v>206</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1670,19 +1707,19 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>141</v>
+        <v>130</v>
+      </c>
+      <c r="E5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>213</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>209</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
-      </c>
-      <c r="N5" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1690,13 +1727,13 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1704,16 +1741,16 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H7" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1721,7 +1758,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1729,19 +1766,16 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>141</v>
+        <v>122</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>210</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
-      </c>
-      <c r="N10" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1749,13 +1783,13 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F11" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
@@ -1769,20 +1803,20 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
       <c r="O12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1790,24 +1824,21 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F13" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G13" t="s">
-        <v>132</v>
+        <v>212</v>
       </c>
       <c r="H13" t="s">
-        <v>150</v>
-      </c>
-      <c r="M13" s="9"/>
-      <c r="N13" t="s">
-        <v>21</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="N13" s="9"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15">
@@ -1822,59 +1853,59 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H16" t="s">
-        <v>172</v>
-      </c>
-      <c r="I16" s="7"/>
+        <v>163</v>
+      </c>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:16">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="F17" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H17" t="s">
-        <v>154</v>
-      </c>
-      <c r="I17" s="7"/>
-      <c r="M17" s="9"/>
+        <v>145</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="N17" s="9"/>
     </row>
     <row r="18" spans="1:16">
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H18" t="s">
-        <v>207</v>
-      </c>
-      <c r="K18" s="8"/>
-      <c r="M18" s="9"/>
+        <v>198</v>
+      </c>
+      <c r="L18" s="8"/>
+      <c r="N18" s="9"/>
     </row>
     <row r="19" spans="1:16">
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="H19" t="s">
-        <v>211</v>
-      </c>
-      <c r="M19" s="9"/>
+        <v>202</v>
+      </c>
+      <c r="N19" s="9"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21">
@@ -1889,14 +1920,14 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="H22" t="s">
-        <v>210</v>
-      </c>
-      <c r="M22" s="9"/>
+        <v>201</v>
+      </c>
+      <c r="N22" s="9"/>
       <c r="P22" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1904,15 +1935,15 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F23" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="H23" t="s">
-        <v>212</v>
-      </c>
-      <c r="M23" s="9"/>
+        <v>203</v>
+      </c>
+      <c r="N23" s="9"/>
     </row>
     <row r="24" spans="1:16">
       <c r="C24" t="s">
@@ -1922,25 +1953,25 @@
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H24" t="s">
-        <v>157</v>
-      </c>
-      <c r="M24" s="9"/>
+        <v>148</v>
+      </c>
+      <c r="N24" s="9"/>
     </row>
     <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="D25" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H25" t="s">
-        <v>157</v>
-      </c>
-      <c r="J25" s="5"/>
-      <c r="M25" s="9"/>
+        <v>148</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="N25" s="9"/>
     </row>
     <row r="27" spans="1:16">
       <c r="A27">
@@ -1955,13 +1986,13 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E28" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="H28" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -1969,116 +2000,116 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F29" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="H29" t="s">
-        <v>213</v>
-      </c>
-      <c r="I29" s="11"/>
-      <c r="M29" s="9"/>
+        <v>204</v>
+      </c>
+      <c r="J29" s="11"/>
+      <c r="N29" s="9"/>
     </row>
     <row r="30" spans="1:16">
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H30" t="s">
-        <v>155</v>
-      </c>
-      <c r="I30" s="11"/>
-      <c r="M30" s="9"/>
+        <v>146</v>
+      </c>
+      <c r="J30" s="11"/>
+      <c r="N30" s="9"/>
     </row>
     <row r="31" spans="1:16">
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H31" t="s">
-        <v>158</v>
-      </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="5"/>
-      <c r="M31" s="9"/>
-    </row>
-    <row r="33" spans="1:13">
+        <v>149</v>
+      </c>
+      <c r="J31" s="7"/>
+      <c r="K31" s="5"/>
+      <c r="N31" s="9"/>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33">
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="H34" t="s">
-        <v>164</v>
-      </c>
-      <c r="M34" s="9"/>
-    </row>
-    <row r="35" spans="1:13">
+        <v>155</v>
+      </c>
+      <c r="N34" s="9"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="H35" t="s">
-        <v>206</v>
-      </c>
-      <c r="M35" s="9"/>
-    </row>
-    <row r="36" spans="1:13">
+        <v>197</v>
+      </c>
+      <c r="N35" s="9"/>
+    </row>
+    <row r="36" spans="1:14">
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="H36" t="s">
-        <v>169</v>
-      </c>
-      <c r="M36" s="9"/>
-    </row>
-    <row r="37" spans="1:13">
+        <v>160</v>
+      </c>
+      <c r="N36" s="9"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H37" t="s">
-        <v>176</v>
-      </c>
-      <c r="I37" s="7"/>
-      <c r="J37" s="5"/>
-      <c r="M37" s="9"/>
-    </row>
-    <row r="38" spans="1:13">
+        <v>167</v>
+      </c>
+      <c r="J37" s="7"/>
+      <c r="K37" s="5"/>
+      <c r="N37" s="9"/>
+    </row>
+    <row r="38" spans="1:14">
       <c r="C38" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D38" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H38" t="s">
-        <v>178</v>
-      </c>
-      <c r="J38" s="5"/>
-      <c r="M38" s="9"/>
-    </row>
-    <row r="40" spans="1:13">
+        <v>169</v>
+      </c>
+      <c r="K38" s="5"/>
+      <c r="N38" s="9"/>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40">
         <v>7</v>
       </c>
@@ -2086,7 +2117,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:14">
       <c r="C41" t="s">
         <v>4</v>
       </c>
@@ -2094,77 +2125,77 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="C42" t="s">
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F42" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="H42" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="H43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="H44" t="s">
-        <v>187</v>
-      </c>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="46" spans="1:13">
+        <v>178</v>
+      </c>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46">
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H47" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F48" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H48" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -2172,10 +2203,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="H49" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -2183,9 +2214,9 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>193</v>
-      </c>
-      <c r="J50" s="5"/>
+        <v>184</v>
+      </c>
+      <c r="K50" s="5"/>
     </row>
     <row r="52" spans="1:15">
       <c r="A52">
@@ -2200,43 +2231,43 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>195</v>
-      </c>
-      <c r="K53" s="8"/>
+        <v>186</v>
+      </c>
+      <c r="L53" s="8"/>
     </row>
     <row r="54" spans="1:15">
       <c r="C54" t="s">
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F54" t="s">
-        <v>204</v>
-      </c>
-      <c r="K54" s="8"/>
+        <v>195</v>
+      </c>
+      <c r="L54" s="8"/>
     </row>
     <row r="55" spans="1:15">
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>22</v>
-      </c>
-      <c r="K55" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="L55" s="8"/>
     </row>
     <row r="56" spans="1:15">
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2268,433 +2299,433 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
         <v>61</v>
-      </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" t="s">
         <v>103</v>
-      </c>
-      <c r="B32" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" t="s">
         <v>88</v>
-      </c>
-      <c r="B40" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" t="s">
         <v>91</v>
-      </c>
-      <c r="B41" t="s">
-        <v>92</v>
-      </c>
-      <c r="C41" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
         <v>96</v>
-      </c>
-      <c r="B44" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish Week 1 Day 3.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="218">
   <si>
     <t>Wk#</t>
   </si>
@@ -543,9 +543,6 @@
     <t>Enumerables, Inheritance</t>
   </si>
   <si>
-    <t>Debugging</t>
-  </si>
-  <si>
     <t>Reading Docs</t>
   </si>
   <si>
@@ -820,6 +817,18 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>Troubleshooting/Debugging</t>
+  </si>
+  <si>
+    <t>Class Rolodex</t>
+  </si>
+  <si>
+    <t>Other assignment options: Tic-tac-toe, Minesweeper</t>
+  </si>
+  <si>
+    <t>Blackjack Advisor</t>
   </si>
 </sst>
 </file>
@@ -980,7 +989,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1024,6 +1033,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1134,7 +1145,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="139">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1204,6 +1215,7 @@
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1270,6 +1282,7 @@
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1604,7 +1617,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1635,37 +1648,37 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F1" t="s">
         <v>118</v>
       </c>
       <c r="G1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" t="s">
         <v>153</v>
       </c>
-      <c r="L1" t="s">
-        <v>154</v>
-      </c>
       <c r="M1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N1" t="s">
         <v>5</v>
       </c>
       <c r="O1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>40</v>
@@ -1684,22 +1697,22 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1707,16 +1720,16 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -1727,13 +1740,22 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="E6" t="s">
+        <v>215</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
+      </c>
+      <c r="H6" t="s">
+        <v>217</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1744,13 +1766,13 @@
         <v>117</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1758,7 +1780,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1766,16 +1788,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>122</v>
+        <v>214</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1786,16 +1811,13 @@
         <v>121</v>
       </c>
       <c r="F11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1803,13 +1825,13 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F12" t="s">
         <v>119</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
@@ -1824,19 +1846,19 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" t="s">
+        <v>211</v>
+      </c>
+      <c r="H13" t="s">
         <v>140</v>
-      </c>
-      <c r="E13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" t="s">
-        <v>212</v>
-      </c>
-      <c r="H13" t="s">
-        <v>141</v>
       </c>
       <c r="N13" s="9"/>
     </row>
@@ -1853,10 +1875,10 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J16" s="7"/>
     </row>
@@ -1865,13 +1887,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J17" s="7"/>
       <c r="N17" s="9"/>
@@ -1881,13 +1903,13 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F18" t="s">
         <v>120</v>
       </c>
       <c r="H18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L18" s="8"/>
       <c r="N18" s="9"/>
@@ -1897,13 +1919,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N19" s="9"/>
     </row>
@@ -1920,14 +1942,14 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N22" s="9"/>
       <c r="P22" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1935,13 +1957,13 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N23" s="9"/>
     </row>
@@ -1953,22 +1975,22 @@
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N24" s="9"/>
     </row>
     <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K25" s="5"/>
       <c r="N25" s="9"/>
@@ -1986,13 +2008,13 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -2000,13 +2022,13 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J29" s="11"/>
       <c r="N29" s="9"/>
@@ -2016,10 +2038,10 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J30" s="11"/>
       <c r="N30" s="9"/>
@@ -2029,10 +2051,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="5"/>
@@ -2043,7 +2065,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2051,10 +2073,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N34" s="9"/>
     </row>
@@ -2063,10 +2085,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H35" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N35" s="9"/>
     </row>
@@ -2075,10 +2097,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N36" s="9"/>
     </row>
@@ -2087,10 +2109,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J37" s="7"/>
       <c r="K37" s="5"/>
@@ -2098,13 +2120,13 @@
     </row>
     <row r="38" spans="1:14">
       <c r="C38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D38" t="s">
+        <v>167</v>
+      </c>
+      <c r="H38" t="s">
         <v>168</v>
-      </c>
-      <c r="H38" t="s">
-        <v>169</v>
       </c>
       <c r="K38" s="5"/>
       <c r="N38" s="9"/>
@@ -2125,7 +2147,7 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2133,13 +2155,13 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2147,10 +2169,10 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
+        <v>175</v>
+      </c>
+      <c r="H43" t="s">
         <v>176</v>
-      </c>
-      <c r="H43" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2158,10 +2180,10 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H44" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K44" s="5"/>
     </row>
@@ -2170,7 +2192,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -2178,10 +2200,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>187</v>
+      </c>
+      <c r="H47" t="s">
         <v>188</v>
-      </c>
-      <c r="H47" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -2189,13 +2211,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F48" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -2203,10 +2225,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -2214,7 +2236,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K50" s="5"/>
     </row>
@@ -2231,7 +2253,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L53" s="8"/>
     </row>
@@ -2240,10 +2262,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L54" s="8"/>
     </row>
@@ -2261,10 +2283,10 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O56" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Add human learning content.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="224">
   <si>
     <t>Wk#</t>
   </si>
@@ -534,9 +534,6 @@
     <t>Human Learning</t>
   </si>
   <si>
-    <t>Estimating</t>
-  </si>
-  <si>
     <t>Googling</t>
   </si>
   <si>
@@ -546,18 +543,12 @@
     <t>Reading Docs</t>
   </si>
   <si>
-    <t>3 ZONES</t>
-  </si>
-  <si>
     <t>Testing, Exceptions</t>
   </si>
   <si>
     <t>Composition, Modules</t>
   </si>
   <si>
-    <t>Pair Programming</t>
-  </si>
-  <si>
     <t>HTML, CSS</t>
   </si>
   <si>
@@ -822,13 +813,40 @@
     <t>Troubleshooting/Debugging</t>
   </si>
   <si>
-    <t>Class Rolodex</t>
-  </si>
-  <si>
     <t>Other assignment options: Tic-tac-toe, Minesweeper</t>
   </si>
   <si>
     <t>Blackjack Advisor</t>
+  </si>
+  <si>
+    <t>Class Contact Info</t>
+  </si>
+  <si>
+    <t>Albums and Artists</t>
+  </si>
+  <si>
+    <t>Durable learning is effortful</t>
+  </si>
+  <si>
+    <t>3 ZONES - Foundation of prior kn.</t>
+  </si>
+  <si>
+    <t>Interleaving learning</t>
+  </si>
+  <si>
+    <t>Estimating is hard</t>
+  </si>
+  <si>
+    <t>Pairing is the shortest feedback cycle</t>
+  </si>
+  <si>
+    <t>Extract key ideas/rules</t>
+  </si>
+  <si>
+    <t>Retrieval practice is better than rereading</t>
+  </si>
+  <si>
+    <t>Elaboration</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1007,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="139">
+  <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1033,6 +1051,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1145,7 +1165,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="139">
+  <cellStyles count="141">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1216,6 +1236,7 @@
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1283,6 +1304,7 @@
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1617,7 +1639,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1648,37 +1670,37 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F1" t="s">
         <v>118</v>
       </c>
       <c r="G1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="M1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N1" t="s">
         <v>5</v>
       </c>
       <c r="O1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>40</v>
@@ -1697,22 +1719,22 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>123</v>
+        <v>217</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1720,16 +1742,16 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -1740,22 +1762,22 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>132</v>
+        <v>214</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>218</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H6" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1765,14 +1787,17 @@
       <c r="D7" t="s">
         <v>117</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>132</v>
+      <c r="E7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>216</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1780,7 +1805,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1788,13 +1813,13 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
@@ -1808,13 +1833,13 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
@@ -1825,13 +1850,13 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>119</v>
+        <v>219</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
@@ -1846,21 +1871,26 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F13" t="s">
-        <v>126</v>
+        <v>222</v>
       </c>
       <c r="G13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="F14" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15">
@@ -1869,16 +1899,22 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
+      <c r="F15" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="16" spans="1:16">
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>143</v>
+      </c>
+      <c r="F16" t="s">
+        <v>221</v>
       </c>
       <c r="H16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="J16" s="7"/>
     </row>
@@ -1887,13 +1923,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J17" s="7"/>
       <c r="N17" s="9"/>
@@ -1903,13 +1939,13 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H18" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L18" s="8"/>
       <c r="N18" s="9"/>
@@ -1919,13 +1955,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F19" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H19" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="N19" s="9"/>
     </row>
@@ -1942,14 +1978,14 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H22" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="N22" s="9"/>
       <c r="P22" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1957,13 +1993,13 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F23" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H23" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N23" s="9"/>
     </row>
@@ -1975,22 +2011,22 @@
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H24" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="N24" s="9"/>
     </row>
     <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D25" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K25" s="5"/>
       <c r="N25" s="9"/>
@@ -2008,13 +2044,13 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H28" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -2022,13 +2058,13 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F29" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H29" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J29" s="11"/>
       <c r="N29" s="9"/>
@@ -2038,10 +2074,10 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="J30" s="11"/>
       <c r="N30" s="9"/>
@@ -2051,10 +2087,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H31" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="5"/>
@@ -2065,7 +2101,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2073,10 +2109,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H34" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="N34" s="9"/>
     </row>
@@ -2085,10 +2121,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H35" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N35" s="9"/>
     </row>
@@ -2097,10 +2133,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H36" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="N36" s="9"/>
     </row>
@@ -2109,10 +2145,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H37" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J37" s="7"/>
       <c r="K37" s="5"/>
@@ -2120,13 +2156,13 @@
     </row>
     <row r="38" spans="1:14">
       <c r="C38" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D38" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H38" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K38" s="5"/>
       <c r="N38" s="9"/>
@@ -2147,7 +2183,7 @@
         <v>11</v>
       </c>
       <c r="H41" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2155,13 +2191,13 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F42" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H42" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2169,10 +2205,10 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H43" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2180,10 +2216,10 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H44" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="K44" s="5"/>
     </row>
@@ -2192,7 +2228,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -2200,10 +2236,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H47" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -2211,13 +2247,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F48" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H48" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -2225,10 +2261,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H49" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -2236,7 +2272,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K50" s="5"/>
     </row>
@@ -2253,7 +2289,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L53" s="8"/>
     </row>
@@ -2262,10 +2298,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F54" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="L54" s="8"/>
     </row>
@@ -2283,10 +2319,10 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="O56" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Begin work on wee k 2.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="225">
   <si>
     <t>Wk#</t>
   </si>
@@ -846,7 +846,10 @@
     <t>Retrieval practice is better than rereading</t>
   </si>
   <si>
-    <t>Elaboration</t>
+    <t>Elaboration is better than repetition</t>
+  </si>
+  <si>
+    <t>Exceptions Article</t>
   </si>
 </sst>
 </file>
@@ -1639,7 +1642,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1798,6 +1801,9 @@
       </c>
       <c r="H7" t="s">
         <v>128</v>
+      </c>
+      <c r="O7" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:16">

</xml_diff>

<commit_message>
Add readings for week 1.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="227">
   <si>
     <t>Wk#</t>
   </si>
@@ -850,6 +850,12 @@
   </si>
   <si>
     <t>Exceptions Article</t>
+  </si>
+  <si>
+    <t>Pro Git 2.2</t>
+  </si>
+  <si>
+    <t>Pro Git 1.3, 2.1</t>
   </si>
 </sst>
 </file>
@@ -1642,7 +1648,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1759,6 +1765,9 @@
       <c r="H5" t="s">
         <v>18</v>
       </c>
+      <c r="O5" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="6" spans="1:16">
       <c r="C6" t="s">
@@ -1778,6 +1787,9 @@
       </c>
       <c r="H6" t="s">
         <v>213</v>
+      </c>
+      <c r="O6" t="s">
+        <v>225</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
Begin work on week 2.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -25,7 +25,7 @@
     <author>Mason</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -122,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -146,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="228">
   <si>
     <t>Wk#</t>
   </si>
@@ -537,15 +537,9 @@
     <t>Googling</t>
   </si>
   <si>
-    <t>Enumerables, Inheritance</t>
-  </si>
-  <si>
     <t>Reading Docs</t>
   </si>
   <si>
-    <t>Testing, Exceptions</t>
-  </si>
-  <si>
     <t>Composition, Modules</t>
   </si>
   <si>
@@ -856,6 +850,15 @@
   </si>
   <si>
     <t>Pro Git 1.3, 2.1</t>
+  </si>
+  <si>
+    <t>Inheritance, Testing</t>
+  </si>
+  <si>
+    <t>Enumerables, Blocks</t>
+  </si>
+  <si>
+    <t>Challenge</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1019,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1060,6 +1063,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1174,7 +1179,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="143">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1246,6 +1251,7 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1314,6 +1320,7 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1644,11 +1651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P56"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1656,16 +1663,17 @@
     <col min="1" max="1" width="5.1640625" customWidth="1"/>
     <col min="3" max="3" width="4.5" customWidth="1"/>
     <col min="4" max="4" width="31.83203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.1640625" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="3.5" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="3"/>
+    <col min="5" max="5" width="19.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="3.5" customWidth="1"/>
+    <col min="16" max="16" width="23.6640625" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1679,43 +1687,46 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
         <v>118</v>
       </c>
-      <c r="G1" t="s">
-        <v>204</v>
-      </c>
       <c r="H1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>210</v>
-      </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="K1" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="L1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M1" t="s">
-        <v>192</v>
+        <v>148</v>
       </c>
       <c r="N1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1723,267 +1734,283 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" t="s">
-        <v>202</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="G4" t="s">
+        <v>215</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" t="s">
+        <v>200</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="H5" t="s">
         <v>203</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="G5" t="s">
-        <v>205</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>18</v>
       </c>
-      <c r="O5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="P5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="E6" t="s">
-        <v>214</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>218</v>
+      <c r="F6" t="s">
+        <v>212</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="H6" t="s">
-        <v>213</v>
-      </c>
-      <c r="O6" t="s">
-        <v>225</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>216</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="I6" t="s">
+        <v>211</v>
+      </c>
+      <c r="P6" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>117</v>
       </c>
-      <c r="E7" t="s">
-        <v>215</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H7" t="s">
-        <v>128</v>
-      </c>
-      <c r="O7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="E7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" t="s">
+        <v>213</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" t="s">
+        <v>126</v>
+      </c>
+      <c r="P7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>211</v>
+        <v>225</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="H10" t="s">
+        <v>209</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="I10" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H11" t="s">
+        <v>226</v>
+      </c>
+      <c r="G11" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>123</v>
-      </c>
-      <c r="F12" t="s">
-        <v>219</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="H12" t="s">
+        <v>121</v>
+      </c>
+      <c r="G12" t="s">
+        <v>217</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" t="s">
         <v>19</v>
       </c>
-      <c r="M12" s="12"/>
-      <c r="O12" t="s">
+      <c r="N12" s="12"/>
+      <c r="P12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F13" t="s">
-        <v>222</v>
+        <v>128</v>
       </c>
       <c r="G13" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="H13" t="s">
-        <v>137</v>
-      </c>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="F14" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+        <v>206</v>
+      </c>
+      <c r="I13" t="s">
+        <v>135</v>
+      </c>
+      <c r="O13" s="9"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="G14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="F15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="G15" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" t="s">
-        <v>221</v>
-      </c>
-      <c r="H16" t="s">
-        <v>159</v>
-      </c>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:16">
+        <v>141</v>
+      </c>
+      <c r="G16" t="s">
+        <v>219</v>
+      </c>
+      <c r="I16" t="s">
+        <v>157</v>
+      </c>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
-      </c>
-      <c r="F17" t="s">
-        <v>152</v>
-      </c>
-      <c r="H17" t="s">
-        <v>141</v>
-      </c>
-      <c r="J17" s="7"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="1:16">
+        <v>177</v>
+      </c>
+      <c r="G17" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="O17" s="9"/>
+    </row>
+    <row r="18" spans="1:17">
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>168</v>
-      </c>
-      <c r="F18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G18" t="s">
         <v>119</v>
       </c>
-      <c r="H18" t="s">
-        <v>194</v>
-      </c>
-      <c r="L18" s="8"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="I18" t="s">
+        <v>192</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="O18" s="9"/>
+    </row>
+    <row r="19" spans="1:17">
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="G19" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" t="s">
         <v>196</v>
       </c>
-      <c r="F19" t="s">
-        <v>131</v>
-      </c>
-      <c r="H19" t="s">
-        <v>198</v>
-      </c>
-      <c r="N19" s="9"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="O19" s="9"/>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>4</v>
       </c>
@@ -1991,65 +2018,65 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>138</v>
-      </c>
-      <c r="H22" t="s">
-        <v>197</v>
-      </c>
-      <c r="N22" s="9"/>
-      <c r="P22" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>136</v>
+      </c>
+      <c r="I22" t="s">
+        <v>195</v>
+      </c>
+      <c r="O22" s="9"/>
+      <c r="Q22" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>139</v>
-      </c>
-      <c r="F23" t="s">
-        <v>154</v>
-      </c>
-      <c r="H23" t="s">
-        <v>199</v>
-      </c>
-      <c r="N23" s="9"/>
-    </row>
-    <row r="24" spans="1:16">
+        <v>137</v>
+      </c>
+      <c r="G23" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" t="s">
+        <v>197</v>
+      </c>
+      <c r="O23" s="9"/>
+    </row>
+    <row r="24" spans="1:17">
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="F24" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" t="s">
-        <v>144</v>
-      </c>
-      <c r="N24" s="9"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="G24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I24" t="s">
+        <v>142</v>
+      </c>
+      <c r="O24" s="9"/>
+    </row>
+    <row r="25" spans="1:17">
       <c r="C25" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H25" t="s">
-        <v>144</v>
-      </c>
-      <c r="K25" s="5"/>
-      <c r="N25" s="9"/>
-    </row>
-    <row r="27" spans="1:16">
+        <v>179</v>
+      </c>
+      <c r="I25" t="s">
+        <v>142</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="O25" s="9"/>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>5</v>
       </c>
@@ -2057,135 +2084,135 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>124</v>
-      </c>
-      <c r="E28" t="s">
-        <v>133</v>
-      </c>
-      <c r="H28" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>122</v>
+      </c>
+      <c r="F28" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>140</v>
-      </c>
-      <c r="F29" t="s">
-        <v>162</v>
-      </c>
-      <c r="H29" t="s">
-        <v>200</v>
-      </c>
-      <c r="J29" s="11"/>
-      <c r="N29" s="9"/>
-    </row>
-    <row r="30" spans="1:16">
+        <v>138</v>
+      </c>
+      <c r="G29" t="s">
+        <v>160</v>
+      </c>
+      <c r="I29" t="s">
+        <v>198</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="O29" s="9"/>
+    </row>
+    <row r="30" spans="1:17">
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
-      </c>
-      <c r="H30" t="s">
-        <v>142</v>
-      </c>
-      <c r="J30" s="11"/>
-      <c r="N30" s="9"/>
-    </row>
-    <row r="31" spans="1:16">
+        <v>144</v>
+      </c>
+      <c r="I30" t="s">
+        <v>140</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="O30" s="9"/>
+    </row>
+    <row r="31" spans="1:17">
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
-      </c>
-      <c r="H31" t="s">
         <v>145</v>
       </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="5"/>
-      <c r="N31" s="9"/>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="I31" t="s">
+        <v>143</v>
+      </c>
+      <c r="K31" s="7"/>
+      <c r="L31" s="5"/>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33">
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
-      </c>
-      <c r="H34" t="s">
-        <v>151</v>
-      </c>
-      <c r="N34" s="9"/>
-    </row>
-    <row r="35" spans="1:14">
+        <v>165</v>
+      </c>
+      <c r="I34" t="s">
+        <v>149</v>
+      </c>
+      <c r="O34" s="9"/>
+    </row>
+    <row r="35" spans="1:15">
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>158</v>
-      </c>
-      <c r="H35" t="s">
-        <v>193</v>
-      </c>
-      <c r="N35" s="9"/>
-    </row>
-    <row r="36" spans="1:14">
+        <v>156</v>
+      </c>
+      <c r="I35" t="s">
+        <v>191</v>
+      </c>
+      <c r="O35" s="9"/>
+    </row>
+    <row r="36" spans="1:15">
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>195</v>
-      </c>
-      <c r="H36" t="s">
-        <v>156</v>
-      </c>
-      <c r="N36" s="9"/>
-    </row>
-    <row r="37" spans="1:14">
+        <v>193</v>
+      </c>
+      <c r="I36" t="s">
+        <v>154</v>
+      </c>
+      <c r="O36" s="9"/>
+    </row>
+    <row r="37" spans="1:15">
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>157</v>
-      </c>
-      <c r="H37" t="s">
+        <v>155</v>
+      </c>
+      <c r="I37" t="s">
+        <v>161</v>
+      </c>
+      <c r="K37" s="7"/>
+      <c r="L37" s="5"/>
+      <c r="O37" s="9"/>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="C38" t="s">
+        <v>158</v>
+      </c>
+      <c r="D38" t="s">
+        <v>162</v>
+      </c>
+      <c r="I38" t="s">
         <v>163</v>
       </c>
-      <c r="J37" s="7"/>
-      <c r="K37" s="5"/>
-      <c r="N37" s="9"/>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="C38" t="s">
-        <v>160</v>
-      </c>
-      <c r="D38" t="s">
-        <v>164</v>
-      </c>
-      <c r="H38" t="s">
-        <v>165</v>
-      </c>
-      <c r="K38" s="5"/>
-      <c r="N38" s="9"/>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="L38" s="5"/>
+      <c r="O38" s="9"/>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40">
         <v>7</v>
       </c>
@@ -2193,108 +2220,108 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:15">
       <c r="C41" t="s">
         <v>4</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
       </c>
-      <c r="H41" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="I41" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="C42" t="s">
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>177</v>
-      </c>
-      <c r="F42" t="s">
-        <v>176</v>
-      </c>
-      <c r="H42" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>175</v>
+      </c>
+      <c r="G42" t="s">
+        <v>174</v>
+      </c>
+      <c r="I42" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>172</v>
-      </c>
-      <c r="H43" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14">
+        <v>170</v>
+      </c>
+      <c r="I43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>175</v>
-      </c>
-      <c r="H44" t="s">
-        <v>174</v>
-      </c>
-      <c r="K44" s="5"/>
-    </row>
-    <row r="46" spans="1:14">
+        <v>173</v>
+      </c>
+      <c r="I44" t="s">
+        <v>172</v>
+      </c>
+      <c r="L44" s="5"/>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46">
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>184</v>
-      </c>
-      <c r="H47" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14">
+        <v>182</v>
+      </c>
+      <c r="I47" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
+        <v>184</v>
+      </c>
+      <c r="G48" t="s">
+        <v>176</v>
+      </c>
+      <c r="I48" t="s">
         <v>186</v>
       </c>
-      <c r="F48" t="s">
-        <v>178</v>
-      </c>
-      <c r="H48" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15">
+    </row>
+    <row r="49" spans="1:16">
       <c r="C49" t="s">
         <v>6</v>
       </c>
       <c r="D49" t="s">
+        <v>185</v>
+      </c>
+      <c r="I49" t="s">
         <v>187</v>
       </c>
-      <c r="H49" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15">
+    </row>
+    <row r="50" spans="1:16">
       <c r="C50" t="s">
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>180</v>
-      </c>
-      <c r="K50" s="5"/>
-    </row>
-    <row r="52" spans="1:15">
+        <v>178</v>
+      </c>
+      <c r="L50" s="5"/>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52">
         <v>9</v>
       </c>
@@ -2302,47 +2329,47 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:16">
       <c r="C53" t="s">
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>182</v>
-      </c>
-      <c r="L53" s="8"/>
-    </row>
-    <row r="54" spans="1:15">
+        <v>180</v>
+      </c>
+      <c r="M53" s="8"/>
+    </row>
+    <row r="54" spans="1:16">
       <c r="C54" t="s">
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F54" t="s">
-        <v>191</v>
-      </c>
-      <c r="L54" s="8"/>
-    </row>
-    <row r="55" spans="1:15">
+        <v>181</v>
+      </c>
+      <c r="G54" t="s">
+        <v>189</v>
+      </c>
+      <c r="M54" s="8"/>
+    </row>
+    <row r="55" spans="1:16">
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55" t="s">
         <v>20</v>
       </c>
-      <c r="L55" s="8"/>
-    </row>
-    <row r="56" spans="1:15">
+      <c r="M55" s="8"/>
+    </row>
+    <row r="56" spans="1:16">
       <c r="C56" t="s">
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>190</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="O56" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="P56" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete week 2 Day 1.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="234">
   <si>
     <t>Wk#</t>
   </si>
@@ -859,6 +859,24 @@
   </si>
   <si>
     <t>Challenge</t>
+  </si>
+  <si>
+    <t>Pro Git 2.5</t>
+  </si>
+  <si>
+    <t>methods</t>
+  </si>
+  <si>
+    <t>loop</t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>hashes</t>
+  </si>
+  <si>
+    <t>Vehicle classes</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1037,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="143">
+  <cellStyleXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1063,6 +1081,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1179,7 +1199,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="143">
+  <cellStyles count="145">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1252,6 +1272,7 @@
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1321,6 +1342,7 @@
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1655,7 +1677,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1856,8 +1878,11 @@
       <c r="D10" t="s">
         <v>225</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>127</v>
+      <c r="E10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" t="s">
+        <v>233</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>209</v>
@@ -1867,6 +1892,9 @@
       </c>
       <c r="I10" t="s">
         <v>19</v>
+      </c>
+      <c r="P10" t="s">
+        <v>228</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>13</v>
@@ -1879,6 +1907,9 @@
       <c r="D11" t="s">
         <v>226</v>
       </c>
+      <c r="E11" t="s">
+        <v>229</v>
+      </c>
       <c r="G11" t="s">
         <v>153</v>
       </c>
@@ -1896,6 +1927,9 @@
       <c r="D12" t="s">
         <v>121</v>
       </c>
+      <c r="E12" t="s">
+        <v>232</v>
+      </c>
       <c r="G12" t="s">
         <v>217</v>
       </c>
@@ -1917,6 +1951,9 @@
       <c r="D13" t="s">
         <v>134</v>
       </c>
+      <c r="E13" t="s">
+        <v>231</v>
+      </c>
       <c r="F13" t="s">
         <v>128</v>
       </c>
@@ -2358,6 +2395,9 @@
         <v>20</v>
       </c>
       <c r="M55" s="8"/>
+      <c r="P55" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="56" spans="1:16">
       <c r="C56" t="s">
@@ -2368,9 +2408,6 @@
       </c>
       <c r="I56" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="P56" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add links to songs.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="234">
   <si>
     <t>Wk#</t>
   </si>
@@ -780,9 +780,6 @@
     <t>Input Statistics</t>
   </si>
   <si>
-    <t>12 Days of Christmas</t>
-  </si>
-  <si>
     <t>Git/Github</t>
   </si>
   <si>
@@ -877,6 +874,9 @@
   </si>
   <si>
     <t>Vehicle classes</t>
+  </si>
+  <si>
+    <t>Monkeys, 12 Days</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1037,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="145">
+  <cellStyleXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1081,6 +1081,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1199,7 +1203,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="145">
+  <cellStyles count="149">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1273,6 +1277,8 @@
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1343,6 +1349,8 @@
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1677,7 +1685,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1709,22 +1717,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G1" t="s">
         <v>118</v>
       </c>
       <c r="H1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K1" t="s">
         <v>164</v>
@@ -1770,7 +1778,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>127</v>
@@ -1793,19 +1801,19 @@
         <v>127</v>
       </c>
       <c r="F5" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1819,22 +1827,22 @@
         <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>199</v>
       </c>
       <c r="I6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1848,10 +1856,10 @@
         <v>127</v>
       </c>
       <c r="F7" t="s">
+        <v>212</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>213</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>214</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>127</v>
@@ -1860,7 +1868,7 @@
         <v>126</v>
       </c>
       <c r="P7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1876,25 +1884,25 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>225</v>
-      </c>
-      <c r="E10" t="s">
-        <v>230</v>
+        <v>224</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I10" t="s">
         <v>19</v>
       </c>
       <c r="P10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>13</v>
@@ -1905,10 +1913,10 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>226</v>
-      </c>
-      <c r="E11" t="s">
-        <v>229</v>
+        <v>225</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="G11" t="s">
         <v>153</v>
@@ -1927,11 +1935,11 @@
       <c r="D12" t="s">
         <v>121</v>
       </c>
-      <c r="E12" t="s">
-        <v>232</v>
+      <c r="E12" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="G12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>127</v>
@@ -1951,17 +1959,17 @@
       <c r="D13" t="s">
         <v>134</v>
       </c>
-      <c r="E13" t="s">
-        <v>231</v>
+      <c r="E13" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="F13" t="s">
         <v>128</v>
       </c>
       <c r="G13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I13" t="s">
         <v>135</v>
@@ -1970,7 +1978,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="G14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1981,7 +1989,7 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1991,8 +1999,11 @@
       <c r="D16" t="s">
         <v>141</v>
       </c>
+      <c r="E16" t="s">
+        <v>229</v>
+      </c>
       <c r="G16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I16" t="s">
         <v>157</v>
@@ -2006,6 +2017,9 @@
       <c r="D17" t="s">
         <v>177</v>
       </c>
+      <c r="E17" t="s">
+        <v>228</v>
+      </c>
       <c r="G17" t="s">
         <v>150</v>
       </c>
@@ -2022,6 +2036,9 @@
       <c r="D18" t="s">
         <v>166</v>
       </c>
+      <c r="E18" t="s">
+        <v>231</v>
+      </c>
       <c r="G18" t="s">
         <v>119</v>
       </c>
@@ -2038,7 +2055,9 @@
       <c r="D19" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="10"/>
+      <c r="E19" t="s">
+        <v>230</v>
+      </c>
       <c r="G19" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
Incorporate changes to Battleship.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -759,9 +759,6 @@
     <t>Authorization, Scope, Delegate</t>
   </si>
   <si>
-    <t>APIs, Regex, JSON</t>
-  </si>
-  <si>
     <t>Consume Github API?</t>
   </si>
   <si>
@@ -852,9 +849,6 @@
     <t>Inheritance, Testing</t>
   </si>
   <si>
-    <t>Enumerables, Blocks</t>
-  </si>
-  <si>
     <t>Challenge</t>
   </si>
   <si>
@@ -877,6 +871,12 @@
   </si>
   <si>
     <t>Monkeys, 12 Days</t>
+  </si>
+  <si>
+    <t>APIs, JSON</t>
+  </si>
+  <si>
+    <t>Regex, Enumerable, and Blocks</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1037,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="149">
+  <cellStyleXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1081,6 +1081,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1203,7 +1207,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="149">
+  <cellStyles count="153">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1279,6 +1283,8 @@
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1351,6 +1357,8 @@
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1684,8 +1692,8 @@
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1717,22 +1725,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G1" t="s">
         <v>118</v>
       </c>
       <c r="H1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K1" t="s">
         <v>164</v>
@@ -1778,13 +1786,13 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>127</v>
       </c>
       <c r="I4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>127</v>
@@ -1801,19 +1809,19 @@
         <v>127</v>
       </c>
       <c r="F5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
       </c>
       <c r="P5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1827,22 +1835,22 @@
         <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1856,10 +1864,10 @@
         <v>127</v>
       </c>
       <c r="F7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>213</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>127</v>
@@ -1868,7 +1876,7 @@
         <v>126</v>
       </c>
       <c r="P7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1884,25 +1892,25 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>232</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>208</v>
+        <v>230</v>
+      </c>
+      <c r="G10" t="s">
+        <v>153</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I10" t="s">
         <v>19</v>
       </c>
       <c r="P10" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>13</v>
@@ -1913,13 +1921,13 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>225</v>
+        <v>121</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>127</v>
       </c>
       <c r="G11" t="s">
-        <v>153</v>
+        <v>207</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>127</v>
@@ -1933,13 +1941,13 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>233</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>127</v>
       </c>
       <c r="G12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>127</v>
@@ -1966,10 +1974,10 @@
         <v>128</v>
       </c>
       <c r="G13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I13" t="s">
         <v>135</v>
@@ -1978,7 +1986,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="G14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1989,7 +1997,7 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -2000,10 +2008,10 @@
         <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I16" t="s">
         <v>157</v>
@@ -2018,7 +2026,7 @@
         <v>177</v>
       </c>
       <c r="E17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G17" t="s">
         <v>150</v>
@@ -2037,7 +2045,7 @@
         <v>166</v>
       </c>
       <c r="E18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G18" t="s">
         <v>119</v>
@@ -2053,16 +2061,16 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="E19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G19" t="s">
         <v>129</v>
       </c>
       <c r="I19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O19" s="9"/>
     </row>
@@ -2082,7 +2090,7 @@
         <v>136</v>
       </c>
       <c r="I22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O22" s="9"/>
       <c r="Q22" s="3" t="s">
@@ -2100,7 +2108,7 @@
         <v>152</v>
       </c>
       <c r="I23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O23" s="9"/>
     </row>
@@ -2165,7 +2173,7 @@
         <v>160</v>
       </c>
       <c r="I29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K29" s="11"/>
       <c r="O29" s="9"/>

</xml_diff>

<commit_message>
Start work on Week 3 Day 1.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="239">
   <si>
     <t>Wk#</t>
   </si>
@@ -225,9 +225,6 @@
     <t>Controllers &amp; APIs</t>
   </si>
   <si>
-    <t>ActiveModel Serializers</t>
-  </si>
-  <si>
     <t>PB&amp;J</t>
   </si>
   <si>
@@ -705,9 +702,6 @@
     <t>TECHNICAL DEBT</t>
   </si>
   <si>
-    <t>ActiveRecord, Unit Testing/Fixtures, Efficiency</t>
-  </si>
-  <si>
     <t>API Security, oAuth</t>
   </si>
   <si>
@@ -867,9 +861,6 @@
     <t>Monkeys, 12 Days</t>
   </si>
   <si>
-    <t>APIs, JSON</t>
-  </si>
-  <si>
     <t>Regex, Enumerable, and Blocks</t>
   </si>
   <si>
@@ -886,6 +877,21 @@
   </si>
   <si>
     <t>Vehicle redux</t>
+  </si>
+  <si>
+    <t>ActiveRecord, Unit Testing</t>
+  </si>
+  <si>
+    <t>ActiveModel Serializers, Seeds/Fixtures</t>
+  </si>
+  <si>
+    <t>Pair Programming Styles</t>
+  </si>
+  <si>
+    <t>Reading APIs, JSON</t>
+  </si>
+  <si>
+    <t>Class Contact redux</t>
   </si>
 </sst>
 </file>
@@ -1729,7 +1735,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1761,43 +1767,43 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1813,25 +1819,25 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1839,25 +1845,25 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1865,28 +1871,28 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="P6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1894,25 +1900,25 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="P7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1920,7 +1926,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1928,26 +1934,26 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J10" s="13"/>
       <c r="P10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>13</v>
@@ -1958,27 +1964,27 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="8"/>
-      <c r="P11" s="4" t="s">
-        <v>127</v>
+      <c r="P11" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1986,27 +1992,27 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" t="s">
         <v>231</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F12" t="s">
-        <v>234</v>
-      </c>
       <c r="G12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J12" s="13"/>
       <c r="L12" s="12"/>
       <c r="P12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2014,27 +2020,27 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G13" t="s">
+        <v>214</v>
+      </c>
+      <c r="H13" t="s">
+        <v>201</v>
+      </c>
+      <c r="I13" t="s">
         <v>133</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F13" t="s">
-        <v>235</v>
-      </c>
-      <c r="G13" t="s">
-        <v>216</v>
-      </c>
-      <c r="H13" t="s">
-        <v>203</v>
-      </c>
-      <c r="I13" t="s">
-        <v>134</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2050,16 +2056,19 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E16" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="F16" t="s">
+        <v>238</v>
       </c>
       <c r="G16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N16" s="7"/>
     </row>
@@ -2068,16 +2077,16 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="E17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="7"/>
@@ -2087,16 +2096,16 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="8"/>
@@ -2107,16 +2116,16 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="E19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M19" s="9"/>
     </row>
@@ -2133,17 +2142,17 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G22" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M22" s="9"/>
       <c r="Q22" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2151,13 +2160,13 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M23" s="9"/>
     </row>
@@ -2166,25 +2175,25 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>235</v>
       </c>
       <c r="G24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:17">
       <c r="C25" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M25" s="9"/>
       <c r="O25" s="5"/>
@@ -2202,13 +2211,13 @@
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2216,13 +2225,13 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I29" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="11"/>
@@ -2232,10 +2241,10 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="11"/>
@@ -2245,10 +2254,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="7"/>
@@ -2259,7 +2268,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2267,10 +2276,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M34" s="9"/>
     </row>
@@ -2279,10 +2288,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2291,10 +2300,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -2303,10 +2312,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M37" s="9"/>
       <c r="N37" s="7"/>
@@ -2314,13 +2323,13 @@
     </row>
     <row r="38" spans="1:15">
       <c r="C38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D38" t="s">
+        <v>160</v>
+      </c>
+      <c r="I38" t="s">
         <v>161</v>
-      </c>
-      <c r="I38" t="s">
-        <v>162</v>
       </c>
       <c r="M38" s="9"/>
       <c r="O38" s="5"/>
@@ -2341,7 +2350,7 @@
         <v>11</v>
       </c>
       <c r="I41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2349,13 +2358,13 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2363,10 +2372,10 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
+        <v>168</v>
+      </c>
+      <c r="I43" t="s">
         <v>169</v>
-      </c>
-      <c r="I43" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -2374,10 +2383,10 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O44" s="5"/>
     </row>
@@ -2386,7 +2395,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -2394,10 +2403,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I47" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -2405,13 +2414,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
+        <v>181</v>
+      </c>
+      <c r="G48" t="s">
+        <v>174</v>
+      </c>
+      <c r="I48" t="s">
         <v>183</v>
-      </c>
-      <c r="G48" t="s">
-        <v>175</v>
-      </c>
-      <c r="I48" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2419,10 +2428,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
+        <v>182</v>
+      </c>
+      <c r="I49" t="s">
         <v>184</v>
-      </c>
-      <c r="I49" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2430,7 +2439,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="O50" s="5"/>
     </row>
@@ -2447,7 +2456,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2456,10 +2465,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G54" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2468,11 +2477,11 @@
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K55" s="8"/>
       <c r="P55" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -2480,10 +2489,10 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2515,433 +2524,433 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
         <v>59</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" t="s">
         <v>106</v>
-      </c>
-      <c r="B29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
         <v>109</v>
-      </c>
-      <c r="B31" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
         <v>102</v>
-      </c>
-      <c r="B33" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
         <v>98</v>
-      </c>
-      <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" t="s">
         <v>111</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" t="s">
         <v>81</v>
-      </c>
-      <c r="B38" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" t="s">
         <v>89</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>90</v>
-      </c>
-      <c r="C41" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" t="s">
         <v>92</v>
       </c>
-      <c r="B43" t="s">
-        <v>93</v>
-      </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
         <v>94</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>95</v>
-      </c>
-      <c r="C44" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" t="s">
         <v>30</v>
-      </c>
-      <c r="B55" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" t="s">
         <v>32</v>
-      </c>
-      <c r="B56" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Week 3 Day 1.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="242">
   <si>
     <t>Wk#</t>
   </si>
@@ -624,9 +624,6 @@
     <t>CULTURE</t>
   </si>
   <si>
-    <t>http://www.vikingcodeschool.com/posts/why-learning-to-code-is-so-damn-hard</t>
-  </si>
-  <si>
     <t>SCARRING w/ AGE</t>
   </si>
   <si>
@@ -642,9 +639,6 @@
     <t>Session, Authentication</t>
   </si>
   <si>
-    <t>Address Book Data Str?</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -792,9 +786,6 @@
     <t>Troubleshooting/Debugging</t>
   </si>
   <si>
-    <t>Other assignment options: Tic-tac-toe, Minesweeper</t>
-  </si>
-  <si>
     <t>Blackjack Advisor</t>
   </si>
   <si>
@@ -846,9 +837,6 @@
     <t>methods</t>
   </si>
   <si>
-    <t>loop</t>
-  </si>
-  <si>
     <t>classes</t>
   </si>
   <si>
@@ -892,6 +880,27 @@
   </si>
   <si>
     <t>Class Contact redux</t>
+  </si>
+  <si>
+    <t>Time Entries Data Struct</t>
+  </si>
+  <si>
+    <t>inheritance</t>
+  </si>
+  <si>
+    <t>composition</t>
+  </si>
+  <si>
+    <t>enumerable</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>RR: Impostor Syndrome</t>
+  </si>
+  <si>
+    <t>Learning Code is Hard</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1011,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1048,6 +1057,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF9C7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1058,7 +1073,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="163">
+  <cellStyleXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1222,8 +1237,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1238,8 +1271,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="163">
+  <cellStyles count="181">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1322,6 +1356,15 @@
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1401,6 +1444,15 @@
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1735,7 +1787,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1767,34 +1819,34 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G1" t="s">
         <v>117</v>
       </c>
       <c r="H1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K1" t="s">
         <v>146</v>
       </c>
       <c r="L1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O1" t="s">
         <v>145</v>
@@ -1828,16 +1880,16 @@
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>126</v>
       </c>
       <c r="I4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1851,19 +1903,19 @@
         <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I5" t="s">
         <v>17</v>
       </c>
       <c r="P5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1877,22 +1929,19 @@
         <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="P6" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1906,10 +1955,10 @@
         <v>126</v>
       </c>
       <c r="F7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>126</v>
@@ -1918,7 +1967,7 @@
         <v>125</v>
       </c>
       <c r="P7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1934,26 +1983,26 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>126</v>
       </c>
       <c r="F10" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="13"/>
       <c r="P10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>13</v>
@@ -1970,10 +2019,10 @@
         <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G11" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>126</v>
@@ -1984,7 +2033,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="8"/>
       <c r="P11" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1992,16 +2041,16 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>126</v>
       </c>
       <c r="F12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G12" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>126</v>
@@ -2026,13 +2075,13 @@
         <v>126</v>
       </c>
       <c r="F13" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G13" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I13" t="s">
         <v>133</v>
@@ -2040,7 +2089,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2059,28 +2108,31 @@
         <v>139</v>
       </c>
       <c r="E16" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G16" t="s">
-        <v>215</v>
+        <v>210</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I16" t="s">
-        <v>155</v>
+        <v>235</v>
       </c>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:16">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G17" t="s">
         <v>148</v>
@@ -2088,48 +2140,53 @@
       <c r="I17" t="s">
         <v>137</v>
       </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="14"/>
       <c r="M17" s="9"/>
       <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="P17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E18" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G18" t="s">
         <v>118</v>
       </c>
       <c r="I18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:16">
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E19" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="G19" t="s">
         <v>127</v>
       </c>
       <c r="I19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M19" s="9"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:16">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2137,45 +2194,54 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:16">
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
         <v>134</v>
       </c>
+      <c r="E22" t="s">
+        <v>237</v>
+      </c>
       <c r="G22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M22" s="9"/>
-      <c r="Q22" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="P22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
         <v>135</v>
       </c>
+      <c r="E23" t="s">
+        <v>238</v>
+      </c>
       <c r="G23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:16">
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>235</v>
+        <v>231</v>
+      </c>
+      <c r="E24" t="s">
+        <v>239</v>
       </c>
       <c r="G24" t="s">
         <v>119</v>
@@ -2185,12 +2251,15 @@
       </c>
       <c r="M24" s="9"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:16">
       <c r="C25" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D25" t="s">
-        <v>176</v>
+        <v>174</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="I25" t="s">
         <v>140</v>
@@ -2198,7 +2267,7 @@
       <c r="M25" s="9"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:16">
       <c r="A27">
         <v>5</v>
       </c>
@@ -2206,7 +2275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:16">
       <c r="C28" t="s">
         <v>4</v>
       </c>
@@ -2220,7 +2289,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:16">
       <c r="C29" t="s">
         <v>5</v>
       </c>
@@ -2228,15 +2297,15 @@
         <v>136</v>
       </c>
       <c r="G29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="11"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:16">
       <c r="C30" t="s">
         <v>6</v>
       </c>
@@ -2249,7 +2318,7 @@
       <c r="M30" s="9"/>
       <c r="N30" s="11"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:16">
       <c r="C31" t="s">
         <v>7</v>
       </c>
@@ -2276,7 +2345,7 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I34" t="s">
         <v>147</v>
@@ -2288,10 +2357,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I35" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2300,10 +2369,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I36" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -2312,10 +2381,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I37" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M37" s="9"/>
       <c r="N37" s="7"/>
@@ -2323,13 +2392,13 @@
     </row>
     <row r="38" spans="1:15">
       <c r="C38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M38" s="9"/>
       <c r="O38" s="5"/>
@@ -2350,7 +2419,7 @@
         <v>11</v>
       </c>
       <c r="I41" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2358,13 +2427,13 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G42" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2372,10 +2441,10 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -2383,10 +2452,10 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="O44" s="5"/>
     </row>
@@ -2395,7 +2464,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -2403,10 +2472,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -2414,13 +2483,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
+        <v>179</v>
+      </c>
+      <c r="G48" t="s">
+        <v>172</v>
+      </c>
+      <c r="I48" t="s">
         <v>181</v>
-      </c>
-      <c r="G48" t="s">
-        <v>174</v>
-      </c>
-      <c r="I48" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2428,10 +2497,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
+        <v>180</v>
+      </c>
+      <c r="I49" t="s">
         <v>182</v>
-      </c>
-      <c r="I49" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2439,7 +2508,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="O50" s="5"/>
     </row>
@@ -2456,7 +2525,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2465,10 +2534,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G54" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2489,7 +2558,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Complete Week 3 Day 2.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -810,12 +810,6 @@
     <t>Extract key ideas/rules</t>
   </si>
   <si>
-    <t>Retrieval practice is better than rereading</t>
-  </si>
-  <si>
-    <t>Elaboration is better than repetition</t>
-  </si>
-  <si>
     <t>Exceptions Article</t>
   </si>
   <si>
@@ -901,6 +895,12 @@
   </si>
   <si>
     <t>Learning Code is Hard</t>
+  </si>
+  <si>
+    <t>Retrieval &gt; rereading, Elaboration &gt; repetition</t>
+  </si>
+  <si>
+    <t>Albums redux</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1073,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="181">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1117,6 +1117,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1273,7 +1275,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="181">
+  <cellStyles count="183">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1365,6 +1367,7 @@
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1453,6 +1456,7 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1787,7 +1791,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1819,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F1" t="s">
         <v>198</v>
@@ -1889,7 +1893,7 @@
         <v>194</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1903,7 +1907,7 @@
         <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>200</v>
@@ -1915,7 +1919,7 @@
         <v>17</v>
       </c>
       <c r="P5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1941,7 +1945,7 @@
         <v>203</v>
       </c>
       <c r="P6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1967,7 +1971,7 @@
         <v>125</v>
       </c>
       <c r="P7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1983,13 +1987,13 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>126</v>
       </c>
       <c r="F10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G10" t="s">
         <v>150</v>
@@ -2002,7 +2006,7 @@
       </c>
       <c r="J10" s="13"/>
       <c r="P10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>13</v>
@@ -2019,7 +2023,7 @@
         <v>126</v>
       </c>
       <c r="F11" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G11" t="s">
         <v>202</v>
@@ -2033,7 +2037,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="8"/>
       <c r="P11" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2041,13 +2045,13 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>126</v>
       </c>
       <c r="F12" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G12" t="s">
         <v>209</v>
@@ -2075,10 +2079,10 @@
         <v>126</v>
       </c>
       <c r="F13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G13" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="H13" t="s">
         <v>199</v>
@@ -2089,7 +2093,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2108,10 +2112,10 @@
         <v>139</v>
       </c>
       <c r="E16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F16" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G16" t="s">
         <v>210</v>
@@ -2120,7 +2124,7 @@
         <v>126</v>
       </c>
       <c r="I16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N16" s="7"/>
     </row>
@@ -2129,10 +2133,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="E17" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="F17" t="s">
+        <v>241</v>
       </c>
       <c r="G17" t="s">
         <v>148</v>
@@ -2145,7 +2152,7 @@
       <c r="M17" s="9"/>
       <c r="N17" s="7"/>
       <c r="P17" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2156,7 +2163,7 @@
         <v>162</v>
       </c>
       <c r="E18" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G18" t="s">
         <v>118</v>
@@ -2173,10 +2180,10 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G19" t="s">
         <v>127</v>
@@ -2202,17 +2209,14 @@
         <v>134</v>
       </c>
       <c r="E22" t="s">
-        <v>237</v>
-      </c>
-      <c r="G22" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="I22" t="s">
         <v>189</v>
       </c>
       <c r="M22" s="9"/>
       <c r="P22" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2223,7 +2227,7 @@
         <v>135</v>
       </c>
       <c r="E23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G23" t="s">
         <v>149</v>
@@ -2238,10 +2242,10 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G24" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Begin work on Week 3 Day 3.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="246">
   <si>
     <t>Wk#</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Models &amp; DB</t>
   </si>
   <si>
-    <t>Know Thy Error Message, know the class of things stored in your variables</t>
-  </si>
-  <si>
     <t>Legacy Code</t>
   </si>
   <si>
@@ -237,9 +234,6 @@
     <t>Skinny Models</t>
   </si>
   <si>
-    <t>http://blog.codeclimate.com/blog/2012/10/17/7-ways-to-decompose-fat-activerecord-models/</t>
-  </si>
-  <si>
     <t>Estimating Games PDF</t>
   </si>
   <si>
@@ -531,9 +525,6 @@
     <t>Human Learning</t>
   </si>
   <si>
-    <t>Googling</t>
-  </si>
-  <si>
     <t>Reading Docs</t>
   </si>
   <si>
@@ -663,9 +654,6 @@
     <t>Asset Pipeline, Workflow Diagrams</t>
   </si>
   <si>
-    <t>Associations, Validations, Seeds/Faker</t>
-  </si>
-  <si>
     <t>Advanced Rails</t>
   </si>
   <si>
@@ -738,21 +726,12 @@
     <t>Teacherbook</t>
   </si>
   <si>
-    <t>Modify existing?</t>
-  </si>
-  <si>
     <t>Authorization, Scope, Delegate</t>
   </si>
   <si>
-    <t>Consume Github API?</t>
-  </si>
-  <si>
     <t>Consume Weather API?</t>
   </si>
   <si>
-    <t>Create Voting API</t>
-  </si>
-  <si>
     <t>Recreate Github Profile</t>
   </si>
   <si>
@@ -901,6 +880,39 @@
   </si>
   <si>
     <t>Albums redux</t>
+  </si>
+  <si>
+    <t>Close a GitHub Issue</t>
+  </si>
+  <si>
+    <t>Create a Voting API</t>
+  </si>
+  <si>
+    <t>Associations, Validations, Faker</t>
+  </si>
+  <si>
+    <t>Assoc/Valid To Coursyl</t>
+  </si>
+  <si>
+    <t>E&amp;D Many-to-many</t>
+  </si>
+  <si>
+    <t>Legacy code</t>
+  </si>
+  <si>
+    <t>How to Google</t>
+  </si>
+  <si>
+    <t>Decompose Fat Models</t>
+  </si>
+  <si>
+    <t>Board Lists</t>
+  </si>
+  <si>
+    <t>Know Thy Error Message</t>
+  </si>
+  <si>
+    <t>Rails Folders</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1085,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1117,6 +1129,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1275,7 +1293,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="189">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1368,6 +1386,9 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1457,6 +1478,9 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1790,8 +1814,8 @@
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1823,43 +1847,43 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="K1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="L1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="O1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="P1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>39</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1875,25 +1899,28 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>223</v>
+        <v>216</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -1901,25 +1928,28 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="F5" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="H5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>213</v>
+        <v>206</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1927,25 +1957,25 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I6" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="P6" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1953,25 +1983,25 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="P7" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1979,7 +2009,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1987,29 +2017,26 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J10" s="13"/>
       <c r="P10" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>13</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2017,27 +2044,27 @@
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G11" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J11" s="13"/>
-      <c r="K11" s="8"/>
+      <c r="K11" s="14"/>
       <c r="P11" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2045,27 +2072,27 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J12" s="13"/>
       <c r="L12" s="12"/>
       <c r="P12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -2073,27 +2100,27 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G13" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="H13" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="I13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2109,169 +2136,181 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F16" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G16" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17">
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E17" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F17" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G17" t="s">
-        <v>148</v>
+        <v>145</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="14"/>
       <c r="M17" s="9"/>
       <c r="N17" s="7"/>
       <c r="P17" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>162</v>
+        <v>237</v>
       </c>
       <c r="E18" t="s">
-        <v>218</v>
+        <v>211</v>
+      </c>
+      <c r="F18" t="s">
+        <v>239</v>
       </c>
       <c r="G18" t="s">
-        <v>118</v>
+        <v>240</v>
       </c>
       <c r="I18" t="s">
-        <v>187</v>
+        <v>238</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E19" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I19" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="M19" s="9"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="C22" t="s">
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E22" t="s">
+        <v>228</v>
+      </c>
+      <c r="G22" t="s">
+        <v>241</v>
+      </c>
+      <c r="I22" t="s">
         <v>235</v>
-      </c>
-      <c r="I22" t="s">
-        <v>189</v>
       </c>
       <c r="M22" s="9"/>
       <c r="P22" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16">
+        <v>232</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E23" t="s">
+        <v>229</v>
+      </c>
+      <c r="G23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I23" t="s">
         <v>236</v>
       </c>
-      <c r="G23" t="s">
-        <v>149</v>
-      </c>
-      <c r="I23" t="s">
-        <v>191</v>
-      </c>
       <c r="M23" s="9"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E24" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M24" s="9"/>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="C25" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M25" s="9"/>
       <c r="O25" s="5"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>5</v>
       </c>
@@ -2279,58 +2318,58 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="C29" t="s">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G29" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I29" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="11"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17">
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="I30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="11"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17">
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="7"/>
@@ -2341,7 +2380,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2349,10 +2388,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I34" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M34" s="9"/>
     </row>
@@ -2361,10 +2400,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="I35" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2373,10 +2412,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I36" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -2385,10 +2424,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="I37" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M37" s="9"/>
       <c r="N37" s="7"/>
@@ -2396,13 +2435,13 @@
     </row>
     <row r="38" spans="1:15">
       <c r="C38" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D38" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="I38" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M38" s="9"/>
       <c r="O38" s="5"/>
@@ -2423,7 +2462,7 @@
         <v>11</v>
       </c>
       <c r="I41" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2431,13 +2470,13 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I42" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2445,10 +2484,10 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I43" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -2456,10 +2495,10 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I44" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="O44" s="5"/>
     </row>
@@ -2468,7 +2507,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -2476,10 +2515,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I47" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -2487,13 +2526,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G48" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="I48" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2501,10 +2540,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="I49" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2512,7 +2551,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="O50" s="5"/>
     </row>
@@ -2521,7 +2560,7 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -2529,7 +2568,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2538,10 +2577,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G54" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2550,11 +2589,11 @@
         <v>6</v>
       </c>
       <c r="D55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K55" s="8"/>
       <c r="P55" s="1" t="s">
-        <v>20</v>
+        <v>242</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -2562,10 +2601,10 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2597,433 +2636,433 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
         <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" t="s">
         <v>100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" t="s">
         <v>85</v>
-      </c>
-      <c r="B40" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="s">
         <v>88</v>
-      </c>
-      <c r="B41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C41" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
         <v>93</v>
-      </c>
-      <c r="B44" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="2" customFormat="1">
       <c r="A54" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B55" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete Week 3 Day 3.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="248">
   <si>
     <t>Wk#</t>
   </si>
@@ -567,9 +567,6 @@
     <t>Gemfile, TDD</t>
   </si>
   <si>
-    <t>Employees and Depts?</t>
-  </si>
-  <si>
     <t>Rails, Web, HTML Verbs</t>
   </si>
   <si>
@@ -882,9 +879,6 @@
     <t>Albums redux</t>
   </si>
   <si>
-    <t>Close a GitHub Issue</t>
-  </si>
-  <si>
     <t>Create a Voting API</t>
   </si>
   <si>
@@ -913,6 +907,18 @@
   </si>
   <si>
     <t>Rails Folders</t>
+  </si>
+  <si>
+    <t>Gitflow</t>
+  </si>
+  <si>
+    <t>Fix git issue?</t>
+  </si>
+  <si>
+    <t>Employees and Depts</t>
+  </si>
+  <si>
+    <t>Close a GitHub Issue?</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1029,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1075,6 +1081,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DFE3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1085,7 +1097,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1275,8 +1287,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1292,8 +1318,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="38" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="203">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1389,6 +1417,13 @@
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1481,6 +1516,13 @@
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1814,8 +1856,8 @@
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1847,43 +1889,43 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G1" t="s">
         <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P1" t="s">
         <v>127</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1908,16 +1950,16 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>115</v>
@@ -1934,22 +1976,22 @@
         <v>123</v>
       </c>
       <c r="F5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -1963,19 +2005,19 @@
         <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -1989,10 +2031,10 @@
         <v>123</v>
       </c>
       <c r="F7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>199</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>123</v>
@@ -2001,7 +2043,7 @@
         <v>122</v>
       </c>
       <c r="P7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2017,26 +2059,27 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="13"/>
+      <c r="M10" s="15"/>
       <c r="P10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2050,10 +2093,10 @@
         <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>123</v>
@@ -2063,8 +2106,9 @@
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="14"/>
+      <c r="M11" s="15"/>
       <c r="P11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2072,16 +2116,16 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>123</v>
@@ -2091,6 +2135,7 @@
       </c>
       <c r="J12" s="13"/>
       <c r="L12" s="12"/>
+      <c r="M12" s="15"/>
       <c r="P12" t="s">
         <v>19</v>
       </c>
@@ -2106,21 +2151,21 @@
         <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G13" t="s">
-        <v>233</v>
-      </c>
-      <c r="H13" t="s">
-        <v>192</v>
+        <v>232</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>130</v>
+        <v>246</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2136,22 +2181,22 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N16" s="7"/>
     </row>
@@ -2160,29 +2205,29 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="14"/>
-      <c r="M17" s="9"/>
+      <c r="M17" s="16"/>
       <c r="N17" s="7"/>
       <c r="P17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2190,39 +2235,42 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
+        <v>235</v>
+      </c>
+      <c r="E18" t="s">
+        <v>210</v>
+      </c>
+      <c r="F18" t="s">
         <v>237</v>
       </c>
-      <c r="E18" t="s">
-        <v>211</v>
-      </c>
-      <c r="F18" t="s">
-        <v>239</v>
-      </c>
       <c r="G18" t="s">
-        <v>240</v>
+        <v>238</v>
+      </c>
+      <c r="H18" t="s">
+        <v>191</v>
       </c>
       <c r="I18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="8"/>
-      <c r="M18" s="9"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:17">
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G19" t="s">
-        <v>124</v>
+        <v>239</v>
       </c>
       <c r="I19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M19" s="9"/>
     </row>
@@ -2239,23 +2287,23 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G22" t="s">
-        <v>241</v>
+        <v>145</v>
       </c>
       <c r="I22" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="M22" s="9"/>
       <c r="P22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2263,17 +2311,18 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G23" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="I23" t="s">
-        <v>236</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="J23" s="13"/>
       <c r="M23" s="9"/>
     </row>
     <row r="24" spans="1:17">
@@ -2281,32 +2330,37 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G24" t="s">
         <v>116</v>
       </c>
       <c r="I24" t="s">
-        <v>137</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="J24" s="13"/>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:17">
       <c r="C25" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="H25" t="s">
+        <v>244</v>
+      </c>
       <c r="I25" t="s">
-        <v>137</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="J25" s="13"/>
       <c r="M25" s="9"/>
       <c r="O25" s="5"/>
     </row>
@@ -2337,13 +2391,13 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="11"/>
@@ -2353,10 +2407,10 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="11"/>
@@ -2366,10 +2420,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="7"/>
@@ -2380,7 +2434,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2388,10 +2442,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M34" s="9"/>
     </row>
@@ -2400,10 +2454,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2412,10 +2466,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -2424,10 +2478,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M37" s="9"/>
       <c r="N37" s="7"/>
@@ -2435,13 +2489,13 @@
     </row>
     <row r="38" spans="1:15">
       <c r="C38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
+        <v>154</v>
+      </c>
+      <c r="I38" t="s">
         <v>155</v>
-      </c>
-      <c r="I38" t="s">
-        <v>156</v>
       </c>
       <c r="M38" s="9"/>
       <c r="O38" s="5"/>
@@ -2461,8 +2515,11 @@
       <c r="D41" t="s">
         <v>11</v>
       </c>
+      <c r="E41" t="s">
+        <v>245</v>
+      </c>
       <c r="I41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2470,13 +2527,16 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>166</v>
+      </c>
+      <c r="E42" t="s">
+        <v>245</v>
       </c>
       <c r="G42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2484,10 +2544,13 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
+        <v>161</v>
+      </c>
+      <c r="E43" t="s">
+        <v>245</v>
+      </c>
+      <c r="I43" t="s">
         <v>162</v>
-      </c>
-      <c r="I43" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -2495,10 +2558,13 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>165</v>
+        <v>164</v>
+      </c>
+      <c r="E44" t="s">
+        <v>245</v>
       </c>
       <c r="I44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O44" s="5"/>
     </row>
@@ -2507,7 +2573,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -2515,10 +2581,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>172</v>
+      </c>
+      <c r="I47" t="s">
         <v>173</v>
-      </c>
-      <c r="I47" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -2526,13 +2592,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G48" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2540,10 +2606,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2551,7 +2617,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O50" s="5"/>
     </row>
@@ -2568,7 +2634,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2577,10 +2643,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2593,7 +2659,7 @@
       </c>
       <c r="K55" s="8"/>
       <c r="P55" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -2601,7 +2667,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Begin work on Week 3 Day 4.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curriculum" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="249">
   <si>
     <t>Wk#</t>
   </si>
@@ -919,6 +919,9 @@
   </si>
   <si>
     <t>Close a GitHub Issue?</t>
+  </si>
+  <si>
+    <t>Design JSON</t>
   </si>
 </sst>
 </file>
@@ -1857,7 +1860,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="C19:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2265,6 +2268,9 @@
       </c>
       <c r="E19" t="s">
         <v>226</v>
+      </c>
+      <c r="F19" t="s">
+        <v>248</v>
       </c>
       <c r="G19" t="s">
         <v>239</v>

</xml_diff>

<commit_message>
Complete work on Week 4 Day 2.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="254">
   <si>
     <t>Wk#</t>
   </si>
@@ -555,9 +555,6 @@
     <t>CSS Reverse Engineer</t>
   </si>
   <si>
-    <t>Personal Site</t>
-  </si>
-  <si>
     <t>Reading/Listening</t>
   </si>
   <si>
@@ -915,9 +912,6 @@
     <t>Employees and Depts</t>
   </si>
   <si>
-    <t>Close a GitHub Issue?</t>
-  </si>
-  <si>
     <t>Design JSON</t>
   </si>
   <si>
@@ -925,6 +919,24 @@
   </si>
   <si>
     <t>Weather Report</t>
+  </si>
+  <si>
+    <t>Fat Models, Skinny Controllers</t>
+  </si>
+  <si>
+    <t>Make a group website</t>
+  </si>
+  <si>
+    <t>GitHub killer</t>
+  </si>
+  <si>
+    <t>API for Voting History</t>
+  </si>
+  <si>
+    <t>Building/Securing APIs</t>
+  </si>
+  <si>
+    <t>Draft Controllers</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1115,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="209">
+  <cellStyleXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1147,6 +1159,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1333,7 +1353,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="38" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="209">
+  <cellStyles count="217">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1439,6 +1459,10 @@
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1541,6 +1565,10 @@
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1875,7 +1903,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1907,43 +1935,43 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1" t="s">
         <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1968,16 +1996,16 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>115</v>
@@ -1994,22 +2022,22 @@
         <v>123</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2023,19 +2051,19 @@
         <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2049,10 +2077,10 @@
         <v>123</v>
       </c>
       <c r="F7" t="s">
+        <v>195</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>196</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>197</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>123</v>
@@ -2061,7 +2089,7 @@
         <v>122</v>
       </c>
       <c r="P7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2069,7 +2097,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -2077,19 +2105,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -2097,7 +2125,7 @@
       <c r="J10" s="13"/>
       <c r="M10" s="15"/>
       <c r="P10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2111,10 +2139,10 @@
         <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>123</v>
@@ -2126,7 +2154,7 @@
       <c r="K11" s="14"/>
       <c r="M11" s="15"/>
       <c r="P11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2134,16 +2162,16 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>123</v>
@@ -2163,27 +2191,27 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2199,22 +2227,22 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N16" s="7"/>
     </row>
@@ -2223,29 +2251,29 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="14"/>
       <c r="M17" s="16"/>
       <c r="N17" s="7"/>
       <c r="P17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2253,22 +2281,22 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
+        <v>233</v>
+      </c>
+      <c r="E18" t="s">
+        <v>208</v>
+      </c>
+      <c r="F18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G18" t="s">
+        <v>236</v>
+      </c>
+      <c r="H18" t="s">
+        <v>189</v>
+      </c>
+      <c r="I18" t="s">
         <v>234</v>
-      </c>
-      <c r="E18" t="s">
-        <v>209</v>
-      </c>
-      <c r="F18" t="s">
-        <v>236</v>
-      </c>
-      <c r="G18" t="s">
-        <v>237</v>
-      </c>
-      <c r="H18" t="s">
-        <v>190</v>
-      </c>
-      <c r="I18" t="s">
-        <v>235</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="8"/>
@@ -2279,13 +2307,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G19" t="s">
         <v>116</v>
@@ -2294,12 +2322,12 @@
         <v>123</v>
       </c>
       <c r="I19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="L19" s="12"/>
       <c r="M19" s="9"/>
       <c r="P19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2315,23 +2343,26 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="F22" t="s">
+        <v>251</v>
       </c>
       <c r="G22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I22" t="s">
-        <v>246</v>
-      </c>
-      <c r="M22" s="9"/>
+        <v>232</v>
+      </c>
+      <c r="N22" s="7"/>
       <c r="P22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2339,54 +2370,62 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="F23" t="s">
+        <v>253</v>
       </c>
       <c r="G23" t="s">
-        <v>124</v>
+        <v>237</v>
       </c>
       <c r="I23" t="s">
-        <v>233</v>
-      </c>
-      <c r="J23" s="13"/>
+        <v>232</v>
+      </c>
       <c r="M23" s="9"/>
+      <c r="P23" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
       <c r="C24" t="s">
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E24" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G24" t="s">
-        <v>238</v>
+        <v>124</v>
       </c>
       <c r="I24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J24" s="13"/>
       <c r="M24" s="9"/>
     </row>
     <row r="25" spans="1:17">
       <c r="C25" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>123</v>
       </c>
       <c r="H25" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J25" s="13"/>
       <c r="M25" s="9"/>
@@ -2408,7 +2447,7 @@
         <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>126</v>
+        <v>249</v>
       </c>
       <c r="I28" t="s">
         <v>125</v>
@@ -2419,13 +2458,16 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="F29" t="s">
+        <v>250</v>
       </c>
       <c r="G29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="11"/>
@@ -2435,10 +2477,10 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M30" s="9"/>
       <c r="N30" s="11"/>
@@ -2448,10 +2490,10 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M31" s="9"/>
       <c r="N31" s="7"/>
@@ -2462,7 +2504,7 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2470,10 +2512,10 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M34" s="9"/>
     </row>
@@ -2482,10 +2524,10 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2494,10 +2536,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M36" s="9"/>
     </row>
@@ -2506,10 +2548,10 @@
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M37" s="9"/>
       <c r="N37" s="7"/>
@@ -2517,13 +2559,13 @@
     </row>
     <row r="38" spans="1:15">
       <c r="C38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D38" t="s">
+        <v>153</v>
+      </c>
+      <c r="I38" t="s">
         <v>154</v>
-      </c>
-      <c r="I38" t="s">
-        <v>155</v>
       </c>
       <c r="M38" s="9"/>
       <c r="O38" s="5"/>
@@ -2544,10 +2586,10 @@
         <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2555,16 +2597,16 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2572,13 +2614,13 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
+        <v>160</v>
+      </c>
+      <c r="E43" t="s">
+        <v>243</v>
+      </c>
+      <c r="I43" t="s">
         <v>161</v>
-      </c>
-      <c r="E43" t="s">
-        <v>244</v>
-      </c>
-      <c r="I43" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -2586,13 +2628,13 @@
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E44" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O44" s="5"/>
     </row>
@@ -2601,7 +2643,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -2609,10 +2651,10 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>171</v>
+      </c>
+      <c r="I47" t="s">
         <v>172</v>
-      </c>
-      <c r="I47" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -2620,13 +2662,13 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G48" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I48" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2634,10 +2676,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2645,7 +2687,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O50" s="5"/>
     </row>
@@ -2662,7 +2704,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2671,10 +2713,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G54" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2687,7 +2729,7 @@
       </c>
       <c r="K55" s="8"/>
       <c r="P55" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -2695,7 +2737,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Complete work on Week 4 Day 3.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curriculum" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="256">
   <si>
     <t>Wk#</t>
   </si>
@@ -723,9 +723,6 @@
     <t>Authorization, Scope, Delegate</t>
   </si>
   <si>
-    <t>Recreate Github Profile</t>
-  </si>
-  <si>
     <t>Markdown, READMEs</t>
   </si>
   <si>
@@ -927,9 +924,6 @@
     <t>Make a group website</t>
   </si>
   <si>
-    <t>GitHub killer</t>
-  </si>
-  <si>
     <t>API for Voting History</t>
   </si>
   <si>
@@ -937,6 +931,18 @@
   </si>
   <si>
     <t>Draft Controllers</t>
+  </si>
+  <si>
+    <t>Mult JSON renders</t>
+  </si>
+  <si>
+    <t>Design branching plan</t>
+  </si>
+  <si>
+    <t>Start on GitHub Profile</t>
+  </si>
+  <si>
+    <t>Recreate GitHub Profile</t>
   </si>
 </sst>
 </file>
@@ -1902,8 +1908,8 @@
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1935,22 +1941,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G1" t="s">
         <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K1" t="s">
         <v>141</v>
@@ -1971,7 +1977,7 @@
         <v>126</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1996,16 +2002,16 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>115</v>
@@ -2022,22 +2028,22 @@
         <v>123</v>
       </c>
       <c r="F5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2051,19 +2057,19 @@
         <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2077,10 +2083,10 @@
         <v>123</v>
       </c>
       <c r="F7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>195</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>196</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>123</v>
@@ -2089,7 +2095,7 @@
         <v>122</v>
       </c>
       <c r="P7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2105,19 +2111,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G10" t="s">
         <v>145</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -2125,7 +2131,7 @@
       <c r="J10" s="13"/>
       <c r="M10" s="15"/>
       <c r="P10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2139,10 +2145,10 @@
         <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>123</v>
@@ -2154,7 +2160,7 @@
       <c r="K11" s="14"/>
       <c r="M11" s="15"/>
       <c r="P11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2162,16 +2168,16 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>123</v>
@@ -2197,21 +2203,21 @@
         <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2230,19 +2236,19 @@
         <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N16" s="7"/>
     </row>
@@ -2251,13 +2257,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G17" t="s">
         <v>143</v>
@@ -2273,7 +2279,7 @@
       <c r="M17" s="16"/>
       <c r="N17" s="7"/>
       <c r="P17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2281,22 +2287,22 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
+        <v>232</v>
+      </c>
+      <c r="E18" t="s">
+        <v>207</v>
+      </c>
+      <c r="F18" t="s">
+        <v>234</v>
+      </c>
+      <c r="G18" t="s">
+        <v>235</v>
+      </c>
+      <c r="H18" t="s">
+        <v>188</v>
+      </c>
+      <c r="I18" t="s">
         <v>233</v>
-      </c>
-      <c r="E18" t="s">
-        <v>208</v>
-      </c>
-      <c r="F18" t="s">
-        <v>235</v>
-      </c>
-      <c r="G18" t="s">
-        <v>236</v>
-      </c>
-      <c r="H18" t="s">
-        <v>189</v>
-      </c>
-      <c r="I18" t="s">
-        <v>234</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="8"/>
@@ -2307,13 +2313,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G19" t="s">
         <v>116</v>
@@ -2322,12 +2328,12 @@
         <v>123</v>
       </c>
       <c r="I19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L19" s="12"/>
       <c r="M19" s="9"/>
       <c r="P19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2346,23 +2352,23 @@
         <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G22" t="s">
         <v>144</v>
       </c>
       <c r="I22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N22" s="7"/>
       <c r="P22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2373,23 +2379,23 @@
         <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M23" s="9"/>
       <c r="P23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2397,10 +2403,13 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E24" t="s">
-        <v>227</v>
+        <v>226</v>
+      </c>
+      <c r="F24" t="s">
+        <v>252</v>
       </c>
       <c r="G24" t="s">
         <v>124</v>
@@ -2421,8 +2430,11 @@
       <c r="E25" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="F25" t="s">
+        <v>253</v>
+      </c>
       <c r="H25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I25" t="s">
         <v>135</v>
@@ -2447,7 +2459,7 @@
         <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I28" t="s">
         <v>125</v>
@@ -2461,13 +2473,13 @@
         <v>131</v>
       </c>
       <c r="F29" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="G29" t="s">
         <v>151</v>
       </c>
       <c r="I29" t="s">
-        <v>182</v>
+        <v>255</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="11"/>
@@ -2586,7 +2598,7 @@
         <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I41" t="s">
         <v>158</v>
@@ -2600,7 +2612,7 @@
         <v>165</v>
       </c>
       <c r="E42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G42" t="s">
         <v>164</v>
@@ -2617,7 +2629,7 @@
         <v>160</v>
       </c>
       <c r="E43" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I43" t="s">
         <v>161</v>
@@ -2631,7 +2643,7 @@
         <v>163</v>
       </c>
       <c r="E44" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I44" t="s">
         <v>162</v>
@@ -2729,7 +2741,7 @@
       </c>
       <c r="K55" s="8"/>
       <c r="P55" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" spans="1:16">

</xml_diff>

<commit_message>
Complete work on Week 4 Day 4.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="260">
   <si>
     <t>Wk#</t>
   </si>
@@ -933,9 +933,6 @@
     <t>Draft Controllers</t>
   </si>
   <si>
-    <t>Mult JSON renders</t>
-  </si>
-  <si>
     <t>Design branching plan</t>
   </si>
   <si>
@@ -943,6 +940,21 @@
   </si>
   <si>
     <t>Recreate GitHub Profile</t>
+  </si>
+  <si>
+    <t>Multi JSON renders</t>
+  </si>
+  <si>
+    <t>RR: Pair Programming</t>
+  </si>
+  <si>
+    <t>Pro Git 2.3, 2.4</t>
+  </si>
+  <si>
+    <t>Pro Git 3.1, 3.2</t>
+  </si>
+  <si>
+    <t>Pro Git 3.3, 3.4</t>
   </si>
 </sst>
 </file>
@@ -1908,8 +1920,8 @@
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I29" sqref="I29"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2251,6 +2263,9 @@
         <v>222</v>
       </c>
       <c r="N16" s="7"/>
+      <c r="P16" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="17" spans="1:17">
       <c r="C17" t="s">
@@ -2307,6 +2322,9 @@
       <c r="J18" s="13"/>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
+      <c r="P18" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="19" spans="1:17">
       <c r="C19" t="s">
@@ -2409,7 +2427,7 @@
         <v>226</v>
       </c>
       <c r="F24" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G24" t="s">
         <v>124</v>
@@ -2419,6 +2437,9 @@
       </c>
       <c r="J24" s="13"/>
       <c r="M24" s="9"/>
+      <c r="P24" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="25" spans="1:17">
       <c r="C25" s="6" t="s">
@@ -2431,7 +2452,7 @@
         <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H25" t="s">
         <v>241</v>
@@ -2442,6 +2463,9 @@
       <c r="J25" s="13"/>
       <c r="M25" s="9"/>
       <c r="O25" s="5"/>
+      <c r="P25" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27">
@@ -2473,13 +2497,13 @@
         <v>131</v>
       </c>
       <c r="F29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G29" t="s">
         <v>151</v>
       </c>
       <c r="I29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M29" s="9"/>
       <c r="N29" s="11"/>

</xml_diff>

<commit_message>
Complete work on Week 5 Day 2.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="261">
   <si>
     <t>Wk#</t>
   </si>
@@ -588,9 +588,6 @@
     <t>Health Tracker</t>
   </si>
   <si>
-    <t>REST, Scaffold</t>
-  </si>
-  <si>
     <t>Helpers/Partials, SCSS/Bootstrap</t>
   </si>
   <si>
@@ -955,6 +952,12 @@
   </si>
   <si>
     <t>Pro Git 3.3, 3.4</t>
+  </si>
+  <si>
+    <t>REST, Scaffold, Integration Tests</t>
+  </si>
+  <si>
+    <t>Pro Git 3.5, 3.6</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1136,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="217">
+  <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1177,6 +1180,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1371,7 +1382,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="38" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="217">
+  <cellStyles count="225">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1481,6 +1492,10 @@
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1587,6 +1602,10 @@
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1920,8 +1939,8 @@
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P25" sqref="P25"/>
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1953,43 +1972,43 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G1" t="s">
         <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
       </c>
       <c r="N1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="O1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P1" t="s">
         <v>126</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2014,16 +2033,16 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>115</v>
@@ -2040,22 +2059,22 @@
         <v>123</v>
       </c>
       <c r="F5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2069,19 +2088,19 @@
         <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2095,10 +2114,10 @@
         <v>123</v>
       </c>
       <c r="F7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>194</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>123</v>
@@ -2107,7 +2126,7 @@
         <v>122</v>
       </c>
       <c r="P7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2123,19 +2142,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -2143,7 +2162,7 @@
       <c r="J10" s="13"/>
       <c r="M10" s="15"/>
       <c r="P10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2157,10 +2176,10 @@
         <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>123</v>
@@ -2172,7 +2191,7 @@
       <c r="K11" s="14"/>
       <c r="M11" s="15"/>
       <c r="P11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2180,16 +2199,16 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>123</v>
@@ -2215,21 +2234,21 @@
         <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2248,23 +2267,23 @@
         <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N16" s="7"/>
       <c r="P16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2272,16 +2291,16 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>123</v>
@@ -2294,7 +2313,7 @@
       <c r="M17" s="16"/>
       <c r="N17" s="7"/>
       <c r="P17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2302,28 +2321,28 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
+        <v>231</v>
+      </c>
+      <c r="E18" t="s">
+        <v>206</v>
+      </c>
+      <c r="F18" t="s">
+        <v>233</v>
+      </c>
+      <c r="G18" t="s">
+        <v>234</v>
+      </c>
+      <c r="H18" t="s">
+        <v>187</v>
+      </c>
+      <c r="I18" t="s">
         <v>232</v>
-      </c>
-      <c r="E18" t="s">
-        <v>207</v>
-      </c>
-      <c r="F18" t="s">
-        <v>234</v>
-      </c>
-      <c r="G18" t="s">
-        <v>235</v>
-      </c>
-      <c r="H18" t="s">
-        <v>188</v>
-      </c>
-      <c r="I18" t="s">
-        <v>233</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
       <c r="P18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2331,13 +2350,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G19" t="s">
         <v>116</v>
@@ -2346,12 +2365,12 @@
         <v>123</v>
       </c>
       <c r="I19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L19" s="12"/>
       <c r="M19" s="9"/>
       <c r="P19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2370,23 +2389,23 @@
         <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N22" s="7"/>
       <c r="P22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2397,23 +2416,23 @@
         <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M23" s="9"/>
       <c r="P23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2421,13 +2440,13 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G24" t="s">
         <v>124</v>
@@ -2438,24 +2457,24 @@
       <c r="J24" s="13"/>
       <c r="M24" s="9"/>
       <c r="P24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="C25" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D25" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I25" t="s">
         <v>135</v>
@@ -2464,7 +2483,7 @@
       <c r="M25" s="9"/>
       <c r="O25" s="5"/>
       <c r="P25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2483,7 +2502,7 @@
         <v>118</v>
       </c>
       <c r="F28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I28" t="s">
         <v>125</v>
@@ -2497,14 +2516,15 @@
         <v>131</v>
       </c>
       <c r="F29" t="s">
+        <v>252</v>
+      </c>
+      <c r="G29" t="s">
+        <v>150</v>
+      </c>
+      <c r="I29" t="s">
         <v>253</v>
       </c>
-      <c r="G29" t="s">
-        <v>151</v>
-      </c>
-      <c r="I29" t="s">
-        <v>254</v>
-      </c>
+      <c r="J29" s="13"/>
       <c r="M29" s="9"/>
       <c r="N29" s="11"/>
     </row>
@@ -2513,7 +2533,7 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>137</v>
+        <v>259</v>
       </c>
       <c r="I30" t="s">
         <v>133</v>
@@ -2526,7 +2546,7 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I31" t="s">
         <v>136</v>
@@ -2535,78 +2555,86 @@
       <c r="N31" s="7"/>
       <c r="O31" s="5"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:16">
       <c r="A33">
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:16">
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M35" s="9"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:16">
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M36" s="9"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:16">
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I37" t="s">
-        <v>152</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="J37" s="13"/>
       <c r="M37" s="9"/>
       <c r="N37" s="7"/>
       <c r="O37" s="5"/>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="P37" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="C38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D38" t="s">
+        <v>152</v>
+      </c>
+      <c r="I38" t="s">
         <v>153</v>
       </c>
-      <c r="I38" t="s">
-        <v>154</v>
-      </c>
+      <c r="J38" s="13"/>
       <c r="M38" s="9"/>
       <c r="O38" s="5"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="P38" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40">
         <v>7</v>
       </c>
@@ -2614,7 +2642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:16">
       <c r="C41" t="s">
         <v>4</v>
       </c>
@@ -2622,89 +2650,89 @@
         <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="C42" t="s">
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E42" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I42" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
+        <v>159</v>
+      </c>
+      <c r="E43" t="s">
+        <v>241</v>
+      </c>
+      <c r="I43" t="s">
         <v>160</v>
       </c>
-      <c r="E43" t="s">
-        <v>242</v>
-      </c>
-      <c r="I43" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
+    </row>
+    <row r="44" spans="1:16">
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O44" s="5"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:16">
       <c r="A46">
         <v>8</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="C47" t="s">
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>170</v>
+      </c>
+      <c r="I47" t="s">
         <v>171</v>
       </c>
-      <c r="I47" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
+    </row>
+    <row r="48" spans="1:16">
       <c r="C48" t="s">
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2712,10 +2740,10 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2723,7 +2751,7 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O50" s="5"/>
     </row>
@@ -2740,7 +2768,7 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2749,10 +2777,10 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G54" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2765,7 +2793,7 @@
       </c>
       <c r="K55" s="8"/>
       <c r="P55" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -2773,7 +2801,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Complete work on Week 5.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="285">
   <si>
     <t>Wk#</t>
   </si>
@@ -663,9 +663,6 @@
     <t>Todo List</t>
   </si>
   <si>
-    <t>JavaScript in Depth</t>
-  </si>
-  <si>
     <t>AUTON/MAST/PURP</t>
   </si>
   <si>
@@ -900,9 +897,6 @@
     <t>Gitflow</t>
   </si>
   <si>
-    <t>Fix git issue?</t>
-  </si>
-  <si>
     <t>Employees and Depts</t>
   </si>
   <si>
@@ -958,13 +952,91 @@
   </si>
   <si>
     <t>Pro Git 3.5, 3.6</t>
+  </si>
+  <si>
+    <t>stash, reset, filter-branch</t>
+  </si>
+  <si>
+    <t>Pro Git 7.7, 7.6</t>
+  </si>
+  <si>
+    <t>discuss ruby</t>
+  </si>
+  <si>
+    <t>html verbs</t>
+  </si>
+  <si>
+    <t>router</t>
+  </si>
+  <si>
+    <t>dev vs prod</t>
+  </si>
+  <si>
+    <t>css selectors</t>
+  </si>
+  <si>
+    <t>html forms</t>
+  </si>
+  <si>
+    <t>fix git issue</t>
+  </si>
+  <si>
+    <t>rest</t>
+  </si>
+  <si>
+    <t>helpers and partials</t>
+  </si>
+  <si>
+    <t>session</t>
+  </si>
+  <si>
+    <t>scope</t>
+  </si>
+  <si>
+    <t>discuss rails</t>
+  </si>
+  <si>
+    <t>javascript</t>
+  </si>
+  <si>
+    <t>jquery</t>
+  </si>
+  <si>
+    <t>Catch-up</t>
+  </si>
+  <si>
+    <t>ajax</t>
+  </si>
+  <si>
+    <t>arel</t>
+  </si>
+  <si>
+    <t>discuss development</t>
+  </si>
+  <si>
+    <t>discuss supporting tech</t>
+  </si>
+  <si>
+    <t>Online voting w/ oAuth/API</t>
+  </si>
+  <si>
+    <t>Upload food photos</t>
+  </si>
+  <si>
+    <t>Add comments to GH Profile</t>
+  </si>
+  <si>
+    <t>DRY out Wallet</t>
+  </si>
+  <si>
+    <t>&amp;&amp;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1067,6 +1139,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1136,7 +1214,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="225">
+  <cellStyleXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1362,8 +1440,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1375,14 +1471,15 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="39"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="38"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="41"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="38" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="41" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="225">
+  <cellStyles count="243">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1496,6 +1593,15 @@
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1606,6 +1712,15 @@
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1939,8 +2054,8 @@
   <dimension ref="A1:Q56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K28" activeCellId="1" sqref="M29 K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1972,28 +2087,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" t="s">
         <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K1" t="s">
         <v>140</v>
       </c>
       <c r="L1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -2008,7 +2123,7 @@
         <v>126</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2033,16 +2148,16 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>115</v>
@@ -2059,22 +2174,22 @@
         <v>123</v>
       </c>
       <c r="F5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2088,19 +2203,19 @@
         <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2114,10 +2229,10 @@
         <v>123</v>
       </c>
       <c r="F7" t="s">
+        <v>192</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>193</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>194</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>123</v>
@@ -2126,7 +2241,7 @@
         <v>122</v>
       </c>
       <c r="P7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2142,27 +2257,27 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G10" t="s">
         <v>144</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="M10" s="15"/>
+      <c r="J10" s="12"/>
+      <c r="M10" s="14"/>
       <c r="P10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2176,10 +2291,10 @@
         <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>123</v>
@@ -2187,11 +2302,11 @@
       <c r="I11" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="14"/>
-      <c r="M11" s="15"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
+      <c r="M11" s="14"/>
       <c r="P11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2199,16 +2314,16 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>123</v>
@@ -2216,9 +2331,9 @@
       <c r="I12" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="13"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="15"/>
+      <c r="J12" s="12"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="14"/>
       <c r="P12" t="s">
         <v>19</v>
       </c>
@@ -2234,21 +2349,21 @@
         <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>242</v>
-      </c>
-      <c r="L13" s="12"/>
+        <v>240</v>
+      </c>
+      <c r="L13" s="11"/>
       <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2267,23 +2382,23 @@
         <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N16" s="7"/>
       <c r="P16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2291,13 +2406,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G17" t="s">
         <v>142</v>
@@ -2308,12 +2423,12 @@
       <c r="I17" t="s">
         <v>132</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="14"/>
-      <c r="M17" s="16"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="13"/>
+      <c r="M17" s="15"/>
       <c r="N17" s="7"/>
       <c r="P17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2321,28 +2436,28 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E18" t="s">
+        <v>205</v>
+      </c>
+      <c r="F18" t="s">
+        <v>232</v>
+      </c>
+      <c r="G18" t="s">
+        <v>233</v>
+      </c>
+      <c r="H18" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18" t="s">
         <v>231</v>
       </c>
-      <c r="E18" t="s">
-        <v>206</v>
-      </c>
-      <c r="F18" t="s">
-        <v>233</v>
-      </c>
-      <c r="G18" t="s">
-        <v>234</v>
-      </c>
-      <c r="H18" t="s">
-        <v>187</v>
-      </c>
-      <c r="I18" t="s">
-        <v>232</v>
-      </c>
-      <c r="J18" s="13"/>
+      <c r="J18" s="12"/>
       <c r="K18" s="8"/>
       <c r="M18" s="9"/>
       <c r="P18" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2350,13 +2465,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G19" t="s">
         <v>116</v>
@@ -2365,12 +2480,12 @@
         <v>123</v>
       </c>
       <c r="I19" t="s">
-        <v>245</v>
-      </c>
-      <c r="L19" s="12"/>
+        <v>243</v>
+      </c>
+      <c r="L19" s="11"/>
       <c r="M19" s="9"/>
       <c r="P19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2389,23 +2504,23 @@
         <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G22" t="s">
         <v>143</v>
       </c>
       <c r="I22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N22" s="7"/>
       <c r="P22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2416,23 +2531,23 @@
         <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F23" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M23" s="9"/>
       <c r="P23" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2440,13 +2555,13 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G24" t="s">
         <v>124</v>
@@ -2454,10 +2569,10 @@
       <c r="I24" t="s">
         <v>135</v>
       </c>
-      <c r="J24" s="13"/>
+      <c r="J24" s="12"/>
       <c r="M24" s="9"/>
       <c r="P24" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2465,25 +2580,25 @@
         <v>149</v>
       </c>
       <c r="D25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H25" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I25" t="s">
         <v>135</v>
       </c>
-      <c r="J25" s="13"/>
+      <c r="J25" s="12"/>
       <c r="M25" s="9"/>
       <c r="O25" s="5"/>
       <c r="P25" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2501,8 +2616,11 @@
       <c r="D28" t="s">
         <v>118</v>
       </c>
+      <c r="E28" t="s">
+        <v>261</v>
+      </c>
       <c r="F28" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I28" t="s">
         <v>125</v>
@@ -2515,31 +2633,42 @@
       <c r="D29" t="s">
         <v>131</v>
       </c>
+      <c r="E29" t="s">
+        <v>262</v>
+      </c>
       <c r="F29" t="s">
-        <v>252</v>
-      </c>
-      <c r="G29" t="s">
-        <v>150</v>
+        <v>250</v>
+      </c>
+      <c r="H29" t="s">
+        <v>259</v>
       </c>
       <c r="I29" t="s">
-        <v>253</v>
-      </c>
-      <c r="J29" s="13"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="11"/>
+        <v>251</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="N29" s="16"/>
+      <c r="P29" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="30" spans="1:17">
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>259</v>
+        <v>257</v>
+      </c>
+      <c r="E30" t="s">
+        <v>263</v>
+      </c>
+      <c r="F30" t="s">
+        <v>282</v>
       </c>
       <c r="I30" t="s">
         <v>133</v>
       </c>
       <c r="M30" s="9"/>
-      <c r="N30" s="11"/>
+      <c r="N30" s="16"/>
     </row>
     <row r="31" spans="1:17">
       <c r="C31" t="s">
@@ -2548,11 +2677,22 @@
       <c r="D31" t="s">
         <v>137</v>
       </c>
+      <c r="E31" t="s">
+        <v>264</v>
+      </c>
+      <c r="F31" t="s">
+        <v>283</v>
+      </c>
+      <c r="G31" t="s">
+        <v>150</v>
+      </c>
       <c r="I31" t="s">
         <v>136</v>
       </c>
       <c r="M31" s="9"/>
-      <c r="N31" s="7"/>
+      <c r="N31" s="17" t="s">
+        <v>284</v>
+      </c>
       <c r="O31" s="5"/>
     </row>
     <row r="33" spans="1:16">
@@ -2570,6 +2710,12 @@
       <c r="D34" t="s">
         <v>155</v>
       </c>
+      <c r="E34" t="s">
+        <v>265</v>
+      </c>
+      <c r="F34" t="s">
+        <v>281</v>
+      </c>
       <c r="I34" t="s">
         <v>141</v>
       </c>
@@ -2582,8 +2728,11 @@
       <c r="D35" t="s">
         <v>147</v>
       </c>
+      <c r="E35" t="s">
+        <v>266</v>
+      </c>
       <c r="I35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M35" s="9"/>
     </row>
@@ -2592,7 +2741,10 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>180</v>
+        <v>179</v>
+      </c>
+      <c r="E36" t="s">
+        <v>268</v>
       </c>
       <c r="I36" t="s">
         <v>145</v>
@@ -2606,15 +2758,18 @@
       <c r="D37" t="s">
         <v>146</v>
       </c>
+      <c r="E37" t="s">
+        <v>269</v>
+      </c>
       <c r="I37" t="s">
         <v>151</v>
       </c>
-      <c r="J37" s="13"/>
+      <c r="J37" s="12"/>
       <c r="M37" s="9"/>
       <c r="N37" s="7"/>
       <c r="O37" s="5"/>
       <c r="P37" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -2624,10 +2779,13 @@
       <c r="D38" t="s">
         <v>152</v>
       </c>
+      <c r="E38" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I38" t="s">
         <v>153</v>
       </c>
-      <c r="J38" s="13"/>
+      <c r="J38" s="12"/>
       <c r="M38" s="9"/>
       <c r="O38" s="5"/>
       <c r="P38" s="4" t="s">
@@ -2650,7 +2808,7 @@
         <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>241</v>
+        <v>270</v>
       </c>
       <c r="I41" t="s">
         <v>157</v>
@@ -2661,13 +2819,13 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E42" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
       <c r="G42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I42" t="s">
         <v>158</v>
@@ -2681,21 +2839,19 @@
         <v>159</v>
       </c>
       <c r="E43" t="s">
-        <v>241</v>
+        <v>267</v>
       </c>
       <c r="I43" t="s">
         <v>160</v>
       </c>
+      <c r="J43" s="12"/>
     </row>
     <row r="44" spans="1:16">
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>162</v>
-      </c>
-      <c r="E44" t="s">
-        <v>241</v>
+        <v>275</v>
       </c>
       <c r="I44" t="s">
         <v>161</v>
@@ -2715,10 +2871,13 @@
         <v>4</v>
       </c>
       <c r="D47" t="s">
+        <v>169</v>
+      </c>
+      <c r="E47" t="s">
+        <v>272</v>
+      </c>
+      <c r="I47" t="s">
         <v>170</v>
-      </c>
-      <c r="I47" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -2726,13 +2885,16 @@
         <v>5</v>
       </c>
       <c r="D48" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="E48" t="s">
+        <v>273</v>
       </c>
       <c r="G48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I48" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -2740,10 +2902,13 @@
         <v>6</v>
       </c>
       <c r="D49" t="s">
-        <v>173</v>
+        <v>172</v>
+      </c>
+      <c r="E49" t="s">
+        <v>274</v>
       </c>
       <c r="I49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -2751,7 +2916,13 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>166</v>
+        <v>165</v>
+      </c>
+      <c r="E50" t="s">
+        <v>276</v>
+      </c>
+      <c r="I50" t="s">
+        <v>280</v>
       </c>
       <c r="O50" s="5"/>
     </row>
@@ -2768,7 +2939,10 @@
         <v>4</v>
       </c>
       <c r="D53" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="E53" t="s">
+        <v>277</v>
       </c>
       <c r="K53" s="8"/>
     </row>
@@ -2777,10 +2951,13 @@
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="E54" t="s">
+        <v>278</v>
       </c>
       <c r="G54" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K54" s="8"/>
     </row>
@@ -2791,9 +2968,12 @@
       <c r="D55" t="s">
         <v>18</v>
       </c>
+      <c r="E55" t="s">
+        <v>279</v>
+      </c>
       <c r="K55" s="8"/>
       <c r="P55" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -2801,7 +2981,7 @@
         <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Complete work on Week 6 Day 2.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -69,7 +69,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Existing Codebase</t>
+TDD</t>
         </r>
       </text>
     </comment>
@@ -117,7 +117,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-TDD</t>
+Existing Codebase</t>
         </r>
       </text>
     </comment>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="290">
   <si>
     <t>Wk#</t>
   </si>
@@ -588,9 +588,6 @@
     <t>Health Tracker</t>
   </si>
   <si>
-    <t>Helpers/Partials, SCSS/Bootstrap</t>
-  </si>
-  <si>
     <t>Intermediate Rails</t>
   </si>
   <si>
@@ -642,9 +639,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Asset Pipeline, Workflow Diagrams</t>
-  </si>
-  <si>
     <t>Advanced Rails</t>
   </si>
   <si>
@@ -1017,9 +1011,6 @@
     <t>discuss supporting tech</t>
   </si>
   <si>
-    <t>Online voting w/ oAuth/API</t>
-  </si>
-  <si>
     <t>Upload food photos</t>
   </si>
   <si>
@@ -1029,7 +1020,31 @@
     <t>DRY out Wallet</t>
   </si>
   <si>
-    <t>&amp;&amp;</t>
+    <t>Helpers/Partials</t>
+  </si>
+  <si>
+    <t>Asset Pipeline, SCSS/Bootstrap</t>
+  </si>
+  <si>
+    <t>Survey Opossum Lab</t>
+  </si>
+  <si>
+    <t>Add menu auth</t>
+  </si>
+  <si>
+    <t>MARKETING YOURSELF</t>
+  </si>
+  <si>
+    <t>RR: Marketing Yourself</t>
+  </si>
+  <si>
+    <t>Ruby Koans</t>
+  </si>
+  <si>
+    <t>Rails vs. Sinatra</t>
+  </si>
+  <si>
+    <t>Take a Ticket</t>
   </si>
 </sst>
 </file>
@@ -1214,7 +1229,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="243">
+  <cellStyleXfs count="303">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1458,8 +1473,68 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1478,8 +1553,9 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="38" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="41" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="243">
+  <cellStyles count="303">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1602,6 +1678,36 @@
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1721,6 +1827,36 @@
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2051,11 +2187,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K28" activeCellId="1" sqref="M29 K28"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2087,43 +2223,43 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G1" t="s">
         <v>115</v>
       </c>
       <c r="H1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K1" t="s">
-        <v>140</v>
+        <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M1" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="N1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P1" t="s">
         <v>126</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2148,16 +2284,16 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>115</v>
@@ -2174,22 +2310,22 @@
         <v>123</v>
       </c>
       <c r="F5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2203,19 +2339,19 @@
         <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="P6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2229,10 +2365,10 @@
         <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>123</v>
@@ -2241,7 +2377,7 @@
         <v>122</v>
       </c>
       <c r="P7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2257,27 +2393,27 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="12"/>
-      <c r="M10" s="14"/>
+      <c r="K10" s="14"/>
       <c r="P10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2291,10 +2427,10 @@
         <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>123</v>
@@ -2303,10 +2439,9 @@
         <v>17</v>
       </c>
       <c r="J11" s="12"/>
-      <c r="K11" s="13"/>
-      <c r="M11" s="14"/>
+      <c r="K11" s="14"/>
       <c r="P11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2314,16 +2449,16 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>123</v>
@@ -2332,8 +2467,8 @@
         <v>17</v>
       </c>
       <c r="J12" s="12"/>
+      <c r="K12" s="14"/>
       <c r="L12" s="11"/>
-      <c r="M12" s="14"/>
       <c r="P12" t="s">
         <v>19</v>
       </c>
@@ -2349,21 +2484,21 @@
         <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G13" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>240</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="K13" s="9"/>
       <c r="L13" s="11"/>
-      <c r="M13" s="9"/>
       <c r="P13" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2382,23 +2517,23 @@
         <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N16" s="7"/>
       <c r="P16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2406,16 +2541,16 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F17" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>123</v>
@@ -2424,11 +2559,11 @@
         <v>132</v>
       </c>
       <c r="J17" s="12"/>
-      <c r="K17" s="13"/>
-      <c r="M17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="M17" s="13"/>
       <c r="N17" s="7"/>
       <c r="P17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2436,28 +2571,28 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
+        <v>228</v>
+      </c>
+      <c r="E18" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" t="s">
         <v>230</v>
       </c>
-      <c r="E18" t="s">
-        <v>205</v>
-      </c>
-      <c r="F18" t="s">
-        <v>232</v>
-      </c>
       <c r="G18" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I18" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J18" s="12"/>
-      <c r="K18" s="8"/>
-      <c r="M18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="M18" s="8"/>
       <c r="P18" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2465,13 +2600,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G19" t="s">
         <v>116</v>
@@ -2480,12 +2615,12 @@
         <v>123</v>
       </c>
       <c r="I19" t="s">
-        <v>243</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="K19" s="9"/>
       <c r="L19" s="11"/>
-      <c r="M19" s="9"/>
       <c r="P19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2504,23 +2639,26 @@
         <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G22" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="N22" s="7"/>
       <c r="P22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2531,23 +2669,27 @@
         <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F23" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G23" t="s">
-        <v>234</v>
+        <v>232</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I23" t="s">
-        <v>229</v>
-      </c>
-      <c r="M23" s="9"/>
+        <v>227</v>
+      </c>
+      <c r="K23" s="9"/>
+      <c r="L23" s="11"/>
       <c r="P23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2555,50 +2697,56 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G24" t="s">
         <v>124</v>
       </c>
+      <c r="H24" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I24" t="s">
         <v>135</v>
       </c>
       <c r="J24" s="12"/>
-      <c r="M24" s="9"/>
+      <c r="K24" s="9"/>
       <c r="P24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="C25" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>249</v>
+        <v>247</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="H25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I25" t="s">
         <v>135</v>
       </c>
       <c r="J25" s="12"/>
-      <c r="M25" s="9"/>
+      <c r="K25" s="9"/>
       <c r="O25" s="5"/>
       <c r="P25" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2617,13 +2765,23 @@
         <v>118</v>
       </c>
       <c r="E28" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F28" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I28" t="s">
         <v>125</v>
+      </c>
+      <c r="M28" s="13"/>
+      <c r="P28" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2634,21 +2792,25 @@
         <v>131</v>
       </c>
       <c r="E29" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F29" t="s">
-        <v>250</v>
+        <v>248</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="H29" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I29" t="s">
-        <v>251</v>
-      </c>
-      <c r="J29" s="12"/>
+        <v>249</v>
+      </c>
+      <c r="J29" s="18"/>
+      <c r="M29" s="13"/>
       <c r="N29" s="16"/>
       <c r="P29" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2656,51 +2818,66 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E30" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F30" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I30" t="s">
         <v>133</v>
       </c>
-      <c r="M30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="11"/>
       <c r="N30" s="16"/>
+      <c r="P30" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="31" spans="1:17">
       <c r="C31" t="s">
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>137</v>
+        <v>281</v>
       </c>
       <c r="E31" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F31" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="G31" t="s">
-        <v>150</v>
+        <v>149</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I31" t="s">
         <v>136</v>
       </c>
-      <c r="M31" s="9"/>
-      <c r="N31" s="17" t="s">
-        <v>284</v>
-      </c>
+      <c r="J31" s="12"/>
+      <c r="K31" s="9"/>
+      <c r="N31" s="7"/>
       <c r="O31" s="5"/>
+      <c r="P31" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33">
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -2708,85 +2885,134 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>282</v>
       </c>
       <c r="E34" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F34" t="s">
-        <v>281</v>
+        <v>278</v>
+      </c>
+      <c r="G34" t="s">
+        <v>285</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I34" t="s">
-        <v>141</v>
-      </c>
-      <c r="M34" s="9"/>
+        <v>140</v>
+      </c>
+      <c r="K34" s="9"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="5"/>
+      <c r="P34" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="35" spans="1:16">
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E35" t="s">
-        <v>266</v>
+        <v>264</v>
+      </c>
+      <c r="F35" t="s">
+        <v>284</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I35" t="s">
-        <v>178</v>
-      </c>
-      <c r="M35" s="9"/>
+        <v>176</v>
+      </c>
+      <c r="K35" s="9"/>
+      <c r="P35" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="36" spans="1:16">
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E36" t="s">
-        <v>268</v>
+        <v>266</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I36" t="s">
-        <v>145</v>
-      </c>
-      <c r="M36" s="9"/>
+        <v>144</v>
+      </c>
+      <c r="K36" s="9"/>
+      <c r="L36" s="11"/>
+      <c r="P36" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="37" spans="1:16">
       <c r="C37" t="s">
         <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E37" t="s">
-        <v>269</v>
+        <v>267</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J37" s="12"/>
-      <c r="M37" s="9"/>
+      <c r="K37" s="9"/>
       <c r="N37" s="7"/>
       <c r="O37" s="5"/>
       <c r="P37" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:16">
       <c r="C38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D38" t="s">
+        <v>151</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I38" t="s">
-        <v>153</v>
-      </c>
       <c r="J38" s="12"/>
-      <c r="M38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="N38" s="17"/>
       <c r="O38" s="5"/>
       <c r="P38" s="4" t="s">
         <v>123</v>
@@ -2805,13 +3031,25 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" t="s">
-        <v>270</v>
-      </c>
-      <c r="I41" t="s">
-        <v>157</v>
+        <v>283</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -2819,171 +3057,221 @@
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>163</v>
+        <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>271</v>
-      </c>
-      <c r="G42" t="s">
-        <v>162</v>
+        <v>268</v>
       </c>
       <c r="I42" t="s">
-        <v>158</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:16">
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E43" t="s">
-        <v>267</v>
+        <v>269</v>
+      </c>
+      <c r="G43" t="s">
+        <v>160</v>
       </c>
       <c r="I43" t="s">
-        <v>160</v>
-      </c>
-      <c r="J43" s="12"/>
+        <v>156</v>
+      </c>
+      <c r="M43" s="8"/>
     </row>
     <row r="44" spans="1:16">
       <c r="C44" t="s">
         <v>7</v>
       </c>
       <c r="D44" t="s">
-        <v>275</v>
+        <v>157</v>
+      </c>
+      <c r="E44" t="s">
+        <v>265</v>
       </c>
       <c r="I44" t="s">
-        <v>161</v>
-      </c>
-      <c r="O44" s="5"/>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="A46">
+        <v>158</v>
+      </c>
+      <c r="J44" s="12"/>
+      <c r="K44" s="9"/>
+      <c r="M44" s="8"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="C45" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" t="s">
+        <v>273</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I45" t="s">
+        <v>159</v>
+      </c>
+      <c r="K45" s="9"/>
+      <c r="O45" s="5"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47">
         <v>8</v>
       </c>
-      <c r="B46" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16">
-      <c r="C47" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" t="s">
-        <v>169</v>
-      </c>
-      <c r="E47" t="s">
-        <v>272</v>
-      </c>
-      <c r="I47" t="s">
-        <v>170</v>
+      <c r="B47" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="1:16">
       <c r="C48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E48" t="s">
-        <v>273</v>
-      </c>
-      <c r="G48" t="s">
-        <v>164</v>
+        <v>270</v>
       </c>
       <c r="I48" t="s">
-        <v>173</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="K48" s="9"/>
     </row>
     <row r="49" spans="1:16">
       <c r="C49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E49" t="s">
-        <v>274</v>
+        <v>271</v>
+      </c>
+      <c r="G49" t="s">
+        <v>162</v>
       </c>
       <c r="I49" t="s">
-        <v>174</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="K49" s="9"/>
+      <c r="O49" s="5"/>
     </row>
     <row r="50" spans="1:16">
       <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>170</v>
+      </c>
+      <c r="E50" t="s">
+        <v>272</v>
+      </c>
+      <c r="I50" t="s">
+        <v>172</v>
+      </c>
+      <c r="K50" s="9"/>
+      <c r="O50" s="5"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="C51" t="s">
         <v>7</v>
       </c>
-      <c r="D50" t="s">
-        <v>165</v>
-      </c>
-      <c r="E50" t="s">
-        <v>276</v>
-      </c>
-      <c r="I50" t="s">
-        <v>280</v>
-      </c>
-      <c r="O50" s="5"/>
-    </row>
-    <row r="52" spans="1:16">
-      <c r="A52">
+      <c r="D51" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" t="s">
+        <v>274</v>
+      </c>
+      <c r="I51" t="s">
+        <v>289</v>
+      </c>
+      <c r="K51" s="9"/>
+      <c r="M51" s="8"/>
+      <c r="O51" s="5"/>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53">
         <v>9</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:16">
-      <c r="C53" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" t="s">
-        <v>167</v>
-      </c>
-      <c r="E53" t="s">
-        <v>277</v>
-      </c>
-      <c r="K53" s="8"/>
     </row>
     <row r="54" spans="1:16">
       <c r="C54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D54" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E54" t="s">
-        <v>278</v>
-      </c>
-      <c r="G54" t="s">
-        <v>176</v>
-      </c>
-      <c r="K54" s="8"/>
+        <v>275</v>
+      </c>
+      <c r="I54" t="s">
+        <v>287</v>
+      </c>
+      <c r="K54" s="14"/>
+      <c r="M54" s="13"/>
+      <c r="P54" s="3" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="55" spans="1:16">
       <c r="C55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="E55" t="s">
-        <v>279</v>
-      </c>
-      <c r="K55" s="8"/>
+        <v>276</v>
+      </c>
+      <c r="G55" t="s">
+        <v>174</v>
+      </c>
+      <c r="I55" t="s">
+        <v>287</v>
+      </c>
+      <c r="K55" s="14"/>
+      <c r="M55" s="13"/>
       <c r="P55" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:16">
       <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" t="s">
+        <v>277</v>
+      </c>
+      <c r="I56" t="s">
+        <v>287</v>
+      </c>
+      <c r="K56" s="14"/>
+      <c r="M56" s="13"/>
+      <c r="P56" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16">
+      <c r="C57" t="s">
         <v>7</v>
       </c>
-      <c r="D56" t="s">
-        <v>175</v>
-      </c>
-      <c r="I56" s="3" t="s">
+      <c r="D57" t="s">
+        <v>173</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="P57" s="3" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete work on Week 7.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="298">
   <si>
     <t>Wk#</t>
   </si>
@@ -1045,6 +1045,30 @@
   </si>
   <si>
     <t>Take a Ticket</t>
+  </si>
+  <si>
+    <t>Add teacherbook controller</t>
+  </si>
+  <si>
+    <t>Many grades at once</t>
+  </si>
+  <si>
+    <t>Eloquent JS Ch. 3, 4</t>
+  </si>
+  <si>
+    <t>Eloquent JS Ch. 5, 12</t>
+  </si>
+  <si>
+    <t>Eloquent JS Ch. 13, 14</t>
+  </si>
+  <si>
+    <t>Eloquent JS Ch. 17, 18</t>
+  </si>
+  <si>
+    <t>Modal doesn't refresh</t>
+  </si>
+  <si>
+    <t>Write, then Discussion</t>
   </si>
 </sst>
 </file>
@@ -1229,7 +1253,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="303">
+  <cellStyleXfs count="323">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1533,8 +1557,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1554,8 +1598,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="41" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="303">
+  <cellStyles count="323">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1708,6 +1753,16 @@
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1857,6 +1912,16 @@
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2190,8 +2255,8 @@
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2946,6 +3011,9 @@
       <c r="E36" t="s">
         <v>266</v>
       </c>
+      <c r="F36" t="s">
+        <v>290</v>
+      </c>
       <c r="G36" s="4" t="s">
         <v>123</v>
       </c>
@@ -2970,6 +3038,9 @@
       </c>
       <c r="E37" t="s">
         <v>267</v>
+      </c>
+      <c r="F37" t="s">
+        <v>291</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>123</v>
@@ -3062,10 +3133,22 @@
       <c r="E42" t="s">
         <v>268</v>
       </c>
+      <c r="F42" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I42" t="s">
         <v>155</v>
       </c>
       <c r="M42" s="8"/>
+      <c r="P42" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="43" spans="1:16">
       <c r="C43" t="s">
@@ -3077,13 +3160,22 @@
       <c r="E43" t="s">
         <v>269</v>
       </c>
+      <c r="F43" s="10" t="s">
+        <v>297</v>
+      </c>
       <c r="G43" t="s">
         <v>160</v>
       </c>
+      <c r="H43" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I43" t="s">
         <v>156</v>
       </c>
       <c r="M43" s="8"/>
+      <c r="P43" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="44" spans="1:16">
       <c r="C44" t="s">
@@ -3095,12 +3187,23 @@
       <c r="E44" t="s">
         <v>265</v>
       </c>
+      <c r="F44" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I44" t="s">
         <v>158</v>
       </c>
-      <c r="J44" s="12"/>
       <c r="K44" s="9"/>
       <c r="M44" s="8"/>
+      <c r="P44" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="45" spans="1:16">
       <c r="C45" t="s">
@@ -3112,11 +3215,24 @@
       <c r="E45" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="F45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I45" t="s">
         <v>159</v>
       </c>
+      <c r="J45" s="19"/>
       <c r="K45" s="9"/>
       <c r="O45" s="5"/>
+      <c r="P45" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="47" spans="1:16">
       <c r="A47">

</xml_diff>

<commit_message>
Complete work on Week 8.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -141,8 +141,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Blue: Data Structure Diagram
-Purple: Workflow Diagram</t>
+Deploy to Heroku</t>
         </r>
       </text>
     </comment>
@@ -166,7 +165,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Deploy to Heroku</t>
+Blue: Data Structure Diagram
+Purple: Workflow Diagram</t>
         </r>
       </text>
     </comment>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="299">
   <si>
     <t>Wk#</t>
   </si>
@@ -1069,6 +1069,9 @@
   </si>
   <si>
     <t>Write, then Discussion</t>
+  </si>
+  <si>
+    <t>Speed up Gradebook</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1243,6 +1246,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1253,7 +1262,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="323">
+  <cellStyleXfs count="337">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1577,8 +1586,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1599,8 +1622,9 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="41" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="323">
+  <cellStyles count="337">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1763,6 +1787,13 @@
     <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1922,6 +1953,13 @@
     <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2255,8 +2293,8 @@
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2315,10 +2353,10 @@
         <v>139</v>
       </c>
       <c r="N1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O1" t="s">
         <v>153</v>
-      </c>
-      <c r="O1" t="s">
-        <v>138</v>
       </c>
       <c r="P1" t="s">
         <v>126</v>
@@ -2596,7 +2634,7 @@
       <c r="I16" t="s">
         <v>218</v>
       </c>
-      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
       <c r="P16" t="s">
         <v>252</v>
       </c>
@@ -2626,7 +2664,7 @@
       <c r="J17" s="12"/>
       <c r="K17" s="15"/>
       <c r="M17" s="13"/>
-      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
       <c r="P17" t="s">
         <v>223</v>
       </c>
@@ -2718,7 +2756,7 @@
       <c r="I22" t="s">
         <v>227</v>
       </c>
-      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
       <c r="P22" t="s">
         <v>224</v>
       </c>
@@ -2809,7 +2847,7 @@
       </c>
       <c r="J25" s="12"/>
       <c r="K25" s="9"/>
-      <c r="O25" s="5"/>
+      <c r="N25" s="5"/>
       <c r="P25" t="s">
         <v>254</v>
       </c>
@@ -2873,7 +2911,7 @@
       </c>
       <c r="J29" s="18"/>
       <c r="M29" s="13"/>
-      <c r="N29" s="16"/>
+      <c r="O29" s="16"/>
       <c r="P29" t="s">
         <v>258</v>
       </c>
@@ -2902,7 +2940,7 @@
       </c>
       <c r="K30" s="9"/>
       <c r="L30" s="11"/>
-      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
       <c r="P30" s="4" t="s">
         <v>123</v>
       </c>
@@ -2931,8 +2969,8 @@
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="9"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="7"/>
       <c r="P31" s="4" t="s">
         <v>123</v>
       </c>
@@ -2968,8 +3006,8 @@
         <v>140</v>
       </c>
       <c r="K34" s="9"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="17"/>
       <c r="P34" t="s">
         <v>286</v>
       </c>
@@ -3053,8 +3091,8 @@
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="9"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="7"/>
       <c r="P37" t="s">
         <v>256</v>
       </c>
@@ -3083,8 +3121,8 @@
       </c>
       <c r="J38" s="12"/>
       <c r="K38" s="9"/>
-      <c r="N38" s="17"/>
-      <c r="O38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="17"/>
       <c r="P38" s="4" t="s">
         <v>123</v>
       </c>
@@ -3229,7 +3267,8 @@
       </c>
       <c r="J45" s="19"/>
       <c r="K45" s="9"/>
-      <c r="O45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="7"/>
       <c r="P45" t="s">
         <v>295</v>
       </c>
@@ -3252,10 +3291,24 @@
       <c r="E48" t="s">
         <v>270</v>
       </c>
+      <c r="F48" t="s">
+        <v>298</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I48" t="s">
         <v>168</v>
       </c>
       <c r="K48" s="9"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="8"/>
+      <c r="P48" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="49" spans="1:16">
       <c r="C49" t="s">
@@ -3270,11 +3323,19 @@
       <c r="G49" t="s">
         <v>162</v>
       </c>
+      <c r="H49" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I49" t="s">
         <v>171</v>
       </c>
       <c r="K49" s="9"/>
-      <c r="O49" s="5"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="5"/>
+      <c r="P49" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="50" spans="1:16">
       <c r="C50" t="s">
@@ -3286,11 +3347,22 @@
       <c r="E50" t="s">
         <v>272</v>
       </c>
+      <c r="G50" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I50" t="s">
         <v>172</v>
       </c>
       <c r="K50" s="9"/>
-      <c r="O50" s="5"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="5"/>
+      <c r="P50" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="51" spans="1:16">
       <c r="C51" t="s">
@@ -3302,12 +3374,24 @@
       <c r="E51" t="s">
         <v>274</v>
       </c>
+      <c r="G51" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I51" t="s">
         <v>289</v>
       </c>
+      <c r="J51" s="20"/>
       <c r="K51" s="9"/>
+      <c r="L51" s="11"/>
       <c r="M51" s="8"/>
-      <c r="O51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="53" spans="1:16">
       <c r="A53">

</xml_diff>

<commit_message>
Add concepts from Ruby Weekly.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Curriculum" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="314">
   <si>
     <t>Wk#</t>
   </si>
@@ -1081,6 +1081,42 @@
   </si>
   <si>
     <t>Log into Gradebook w/ Facebook</t>
+  </si>
+  <si>
+    <t>RR: Agile Communication</t>
+  </si>
+  <si>
+    <t>Hiring Apprentices</t>
+  </si>
+  <si>
+    <t>RR: Hacking Education</t>
+  </si>
+  <si>
+    <t>RR: The Science of Software</t>
+  </si>
+  <si>
+    <t>Rails Guide on SQL</t>
+  </si>
+  <si>
+    <t>RR: Technology Radar</t>
+  </si>
+  <si>
+    <t>RR: Estimation</t>
+  </si>
+  <si>
+    <t>RR: Technical Debt</t>
+  </si>
+  <si>
+    <t>RR: When to use Modules</t>
+  </si>
+  <si>
+    <t>RR: Ruby Antipatterns</t>
+  </si>
+  <si>
+    <t>Human Learning/Agile</t>
+  </si>
+  <si>
+    <t>Agile Practices</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1307,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="337">
+  <cellStyleXfs count="339">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1315,6 +1351,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1633,7 +1671,7 @@
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="337">
+  <cellStyles count="339">
     <cellStyle name="20% - Accent1" xfId="40" builtinId="30"/>
     <cellStyle name="40% - Accent4" xfId="41" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="42" builtinId="51"/>
@@ -1803,6 +1841,7 @@
     <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="37" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -1969,6 +2008,7 @@
     <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="39" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2301,9 +2341,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2341,7 +2381,7 @@
         <v>183</v>
       </c>
       <c r="G1" t="s">
-        <v>115</v>
+        <v>312</v>
       </c>
       <c r="H1" t="s">
         <v>180</v>
@@ -2526,6 +2566,9 @@
       <c r="K10" s="14"/>
       <c r="P10" t="s">
         <v>201</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2892,8 +2935,8 @@
         <v>125</v>
       </c>
       <c r="M28" s="13"/>
-      <c r="P28" s="4" t="s">
-        <v>123</v>
+      <c r="P28" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2950,8 +2993,8 @@
       <c r="K30" s="9"/>
       <c r="L30" s="11"/>
       <c r="O30" s="16"/>
-      <c r="P30" s="4" t="s">
-        <v>123</v>
+      <c r="P30" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -2980,8 +3023,8 @@
       <c r="K31" s="9"/>
       <c r="N31" s="5"/>
       <c r="O31" s="7"/>
-      <c r="P31" s="4" t="s">
-        <v>123</v>
+      <c r="P31" s="10" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -3044,8 +3087,8 @@
         <v>176</v>
       </c>
       <c r="K35" s="9"/>
-      <c r="P35" s="4" t="s">
-        <v>123</v>
+      <c r="P35" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -3072,8 +3115,8 @@
       </c>
       <c r="K36" s="9"/>
       <c r="L36" s="11"/>
-      <c r="P36" s="4" t="s">
-        <v>123</v>
+      <c r="P36" s="10" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3315,8 +3358,8 @@
       <c r="K48" s="9"/>
       <c r="L48" s="11"/>
       <c r="M48" s="8"/>
-      <c r="P48" s="4" t="s">
-        <v>123</v>
+      <c r="P48" s="10" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -3345,8 +3388,8 @@
       <c r="L49" s="11"/>
       <c r="M49" s="8"/>
       <c r="N49" s="5"/>
-      <c r="P49" s="4" t="s">
-        <v>123</v>
+      <c r="P49" s="10" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -3375,8 +3418,8 @@
       <c r="L50" s="11"/>
       <c r="M50" s="8"/>
       <c r="N50" s="5"/>
-      <c r="P50" s="4" t="s">
-        <v>123</v>
+      <c r="P50" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -3407,8 +3450,8 @@
       <c r="M51" s="8"/>
       <c r="N51" s="5"/>
       <c r="O51" s="17"/>
-      <c r="P51" s="4" t="s">
-        <v>123</v>
+      <c r="P51" s="10" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -3429,13 +3472,16 @@
       <c r="E54" t="s">
         <v>275</v>
       </c>
+      <c r="G54" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I54" t="s">
         <v>287</v>
       </c>
       <c r="K54" s="14"/>
       <c r="M54" s="13"/>
-      <c r="P54" s="3" t="s">
-        <v>123</v>
+      <c r="P54" s="1" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -3470,6 +3516,9 @@
       <c r="E56" t="s">
         <v>277</v>
       </c>
+      <c r="G56" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="I56" t="s">
         <v>287</v>
       </c>
@@ -3485,6 +3534,12 @@
       </c>
       <c r="D57" t="s">
         <v>173</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
Integrate week 8 project.
</commit_message>
<xml_diff>
--- a/during/overview.xlsx
+++ b/during/overview.xlsx
@@ -681,9 +681,6 @@
     <t>SQL, AREL, Indices</t>
   </si>
   <si>
-    <t>Database Optimizations</t>
-  </si>
-  <si>
     <t>Mailer, Delayed Job</t>
   </si>
   <si>
@@ -1035,9 +1032,6 @@
     <t>Rails vs. Sinatra</t>
   </si>
   <si>
-    <t>Take a Ticket</t>
-  </si>
-  <si>
     <t>Add teacherbook controller</t>
   </si>
   <si>
@@ -1117,6 +1111,12 @@
   </si>
   <si>
     <t>discuss html and http</t>
+  </si>
+  <si>
+    <t>SQL to Rails Queries</t>
+  </si>
+  <si>
+    <t>Gradebook Tickets</t>
   </si>
 </sst>
 </file>
@@ -2346,8 +2346,8 @@
   <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2379,28 +2379,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K1" t="s">
         <v>5</v>
       </c>
       <c r="L1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1" t="s">
         <v>139</v>
@@ -2415,7 +2415,7 @@
         <v>126</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -2440,16 +2440,16 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>115</v>
@@ -2466,22 +2466,22 @@
         <v>123</v>
       </c>
       <c r="F5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I5" t="s">
         <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -2495,19 +2495,19 @@
         <v>123</v>
       </c>
       <c r="F6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2521,10 +2521,10 @@
         <v>123</v>
       </c>
       <c r="F7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>123</v>
@@ -2533,7 +2533,7 @@
         <v>122</v>
       </c>
       <c r="P7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -2549,19 +2549,19 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G10" t="s">
         <v>143</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I10" t="s">
         <v>17</v>
@@ -2569,10 +2569,10 @@
       <c r="J10" s="12"/>
       <c r="K10" s="14"/>
       <c r="P10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -2586,10 +2586,10 @@
         <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>123</v>
@@ -2600,7 +2600,7 @@
       <c r="J11" s="12"/>
       <c r="K11" s="14"/>
       <c r="P11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -2608,16 +2608,16 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>123</v>
       </c>
       <c r="F12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>123</v>
@@ -2643,21 +2643,21 @@
         <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="11"/>
       <c r="P13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -2676,23 +2676,23 @@
         <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F16" t="s">
+        <v>216</v>
+      </c>
+      <c r="G16" t="s">
+        <v>194</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" t="s">
         <v>217</v>
-      </c>
-      <c r="G16" t="s">
-        <v>195</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="I16" t="s">
-        <v>218</v>
       </c>
       <c r="O16" s="7"/>
       <c r="P16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -2700,13 +2700,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G17" t="s">
         <v>141</v>
@@ -2722,7 +2722,7 @@
       <c r="M17" s="13"/>
       <c r="O17" s="7"/>
       <c r="P17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -2730,28 +2730,28 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
+        <v>227</v>
+      </c>
+      <c r="E18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F18" t="s">
+        <v>229</v>
+      </c>
+      <c r="G18" t="s">
+        <v>230</v>
+      </c>
+      <c r="H18" t="s">
+        <v>183</v>
+      </c>
+      <c r="I18" t="s">
         <v>228</v>
-      </c>
-      <c r="E18" t="s">
-        <v>203</v>
-      </c>
-      <c r="F18" t="s">
-        <v>230</v>
-      </c>
-      <c r="G18" t="s">
-        <v>231</v>
-      </c>
-      <c r="H18" t="s">
-        <v>184</v>
-      </c>
-      <c r="I18" t="s">
-        <v>229</v>
       </c>
       <c r="J18" s="12"/>
       <c r="K18" s="9"/>
       <c r="M18" s="8"/>
       <c r="P18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -2759,13 +2759,13 @@
         <v>7</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G19" t="s">
         <v>116</v>
@@ -2774,12 +2774,12 @@
         <v>123</v>
       </c>
       <c r="I19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="11"/>
       <c r="P19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2798,10 +2798,10 @@
         <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G22" t="s">
         <v>142</v>
@@ -2810,14 +2810,14 @@
         <v>123</v>
       </c>
       <c r="I22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O22" s="7"/>
       <c r="P22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -2828,27 +2828,27 @@
         <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="11"/>
       <c r="P23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -2856,13 +2856,13 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G24" t="s">
         <v>124</v>
@@ -2876,7 +2876,7 @@
       <c r="J24" s="12"/>
       <c r="K24" s="9"/>
       <c r="P24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -2890,13 +2890,13 @@
         <v>123</v>
       </c>
       <c r="F25" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>123</v>
       </c>
       <c r="H25" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I25" t="s">
         <v>135</v>
@@ -2905,7 +2905,7 @@
       <c r="K25" s="9"/>
       <c r="N25" s="5"/>
       <c r="P25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2924,10 +2924,10 @@
         <v>118</v>
       </c>
       <c r="E28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>123</v>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="M28" s="13"/>
       <c r="P28" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2951,25 +2951,25 @@
         <v>131</v>
       </c>
       <c r="E29" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F29" t="s">
+        <v>247</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H29" t="s">
+        <v>256</v>
+      </c>
+      <c r="I29" t="s">
         <v>248</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="H29" t="s">
-        <v>257</v>
-      </c>
-      <c r="I29" t="s">
-        <v>249</v>
       </c>
       <c r="J29" s="18"/>
       <c r="M29" s="13"/>
       <c r="O29" s="16"/>
       <c r="P29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -2977,13 +2977,13 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>123</v>
@@ -2998,7 +2998,7 @@
       <c r="L30" s="11"/>
       <c r="O30" s="16"/>
       <c r="P30" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -3006,13 +3006,13 @@
         <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G31" t="s">
         <v>149</v>
@@ -3028,7 +3028,7 @@
       <c r="N31" s="5"/>
       <c r="O31" s="7"/>
       <c r="P31" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -3044,16 +3044,16 @@
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E34" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G34" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>123</v>
@@ -3065,7 +3065,7 @@
       <c r="N34" s="5"/>
       <c r="O34" s="17"/>
       <c r="P34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -3076,10 +3076,10 @@
         <v>146</v>
       </c>
       <c r="E35" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>123</v>
@@ -3088,11 +3088,11 @@
         <v>123</v>
       </c>
       <c r="I35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K35" s="9"/>
       <c r="P35" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -3100,13 +3100,13 @@
         <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E36" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F36" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>123</v>
@@ -3120,7 +3120,7 @@
       <c r="K36" s="9"/>
       <c r="L36" s="11"/>
       <c r="P36" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3131,10 +3131,10 @@
         <v>145</v>
       </c>
       <c r="E37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F37" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>123</v>
@@ -3150,7 +3150,7 @@
       <c r="N37" s="5"/>
       <c r="O37" s="7"/>
       <c r="P37" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -3196,7 +3196,7 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>123</v>
@@ -3225,10 +3225,10 @@
         <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>123</v>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="M42" s="8"/>
       <c r="P42" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3252,10 +3252,10 @@
         <v>161</v>
       </c>
       <c r="E43" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G43" t="s">
         <v>160</v>
@@ -3268,7 +3268,7 @@
       </c>
       <c r="M43" s="8"/>
       <c r="P43" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3279,10 +3279,10 @@
         <v>157</v>
       </c>
       <c r="E44" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>123</v>
@@ -3296,7 +3296,7 @@
       <c r="K44" s="9"/>
       <c r="M44" s="8"/>
       <c r="P44" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -3304,7 +3304,7 @@
         <v>147</v>
       </c>
       <c r="D45" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>123</v>
@@ -3326,7 +3326,7 @@
       <c r="N45" s="5"/>
       <c r="O45" s="7"/>
       <c r="P45" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -3345,10 +3345,10 @@
         <v>167</v>
       </c>
       <c r="E48" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F48" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>123</v>
@@ -3357,13 +3357,13 @@
         <v>123</v>
       </c>
       <c r="I48" t="s">
-        <v>168</v>
+        <v>312</v>
       </c>
       <c r="K48" s="9"/>
       <c r="L48" s="11"/>
       <c r="M48" s="8"/>
       <c r="P48" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -3371,13 +3371,13 @@
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E49" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F49" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G49" t="s">
         <v>162</v>
@@ -3386,14 +3386,14 @@
         <v>123</v>
       </c>
       <c r="I49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="11"/>
       <c r="M49" s="8"/>
       <c r="N49" s="5"/>
       <c r="P49" s="10" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -3401,13 +3401,13 @@
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E50" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F50" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>123</v>
@@ -3416,14 +3416,14 @@
         <v>123</v>
       </c>
       <c r="I50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K50" s="9"/>
       <c r="L50" s="11"/>
       <c r="M50" s="8"/>
       <c r="N50" s="5"/>
       <c r="P50" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -3434,10 +3434,10 @@
         <v>163</v>
       </c>
       <c r="E51" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F51" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>123</v>
@@ -3446,7 +3446,7 @@
         <v>123</v>
       </c>
       <c r="I51" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
       <c r="J51" s="20"/>
       <c r="K51" s="9"/>
@@ -3455,7 +3455,7 @@
       <c r="N51" s="5"/>
       <c r="O51" s="17"/>
       <c r="P51" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -3474,18 +3474,18 @@
         <v>165</v>
       </c>
       <c r="E54" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I54" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K54" s="14"/>
       <c r="M54" s="13"/>
       <c r="P54" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -3496,18 +3496,18 @@
         <v>166</v>
       </c>
       <c r="E55" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I55" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K55" s="14"/>
       <c r="M55" s="13"/>
       <c r="P55" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -3518,18 +3518,18 @@
         <v>18</v>
       </c>
       <c r="E56" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>123</v>
       </c>
       <c r="I56" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K56" s="14"/>
       <c r="M56" s="13"/>
       <c r="P56" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -3537,7 +3537,7 @@
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>123</v>

</xml_diff>